<commit_message>
Added a patient and scenario for core/skin temperatures during exercise. Updated .xlsx and .md documentation for validation scenario
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/EnergyEnvironmentValidation.xlsx
+++ b/share/doc/validation/Scenarios/EnergyEnvironmentValidation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntatum\BioGearsCMake\core\share\doc\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="24720" windowHeight="10965" activeTab="9"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="24720" windowHeight="10965" firstSheet="4" activeTab="10"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -17,15 +22,16 @@
     <sheet name="ExerciseVO2max" sheetId="8" r:id="rId8"/>
     <sheet name="ExerciseSustained" sheetId="16" r:id="rId9"/>
     <sheet name="Starvation" sheetId="10" r:id="rId10"/>
-    <sheet name="Dehydration" sheetId="11" r:id="rId11"/>
-    <sheet name="SarinNerveAgent" sheetId="15" r:id="rId12"/>
+    <sheet name="ExerciseTemperatureTest" sheetId="17" r:id="rId11"/>
+    <sheet name="Dehydration" sheetId="11" r:id="rId12"/>
+    <sheet name="SarinNerveAgent" sheetId="15" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1622" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="289">
   <si>
     <t>Action</t>
   </si>
@@ -887,11 +893,29 @@
   <si>
     <t>%Hepatic Gluconeogenesis Rate (g/day)</t>
   </si>
+  <si>
+    <t>Working at about 50% of VO2 max</t>
+  </si>
+  <si>
+    <t>Skin Temperature</t>
+  </si>
+  <si>
+    <t>Core Temperature</t>
+  </si>
+  <si>
+    <t>Exercise in 37 degC</t>
+  </si>
+  <si>
+    <t>38.7 degC @cite tsuji2011effect</t>
+  </si>
+  <si>
+    <t>35.7 degC @cite tsuji2011effect</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1935,7 +1959,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1970,7 +1994,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2741,7 +2765,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:AH9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
@@ -2784,7 +2808,7 @@
     <col min="35" max="16384" width="9.140625" style="69"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="71" t="s">
         <v>47</v>
       </c>
@@ -2987,7 +3011,7 @@
       </c>
       <c r="AH3" s="75"/>
     </row>
-    <row r="4" spans="1:34" ht="90" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:34" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A4" s="71" t="s">
         <v>47</v>
       </c>
@@ -3101,6 +3125,144 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:M4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="42" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="42" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="I2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="40" t="s">
+        <v>284</v>
+      </c>
+      <c r="K2" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="40" t="s">
+        <v>285</v>
+      </c>
+      <c r="M2" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="28" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="31" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>286</v>
+      </c>
+      <c r="C4" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="11" t="s">
+        <v>283</v>
+      </c>
+      <c r="E4" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="11">
+        <v>2400</v>
+      </c>
+      <c r="G4" s="31" t="s">
+        <v>47</v>
+      </c>
+      <c r="H4" s="11">
+        <v>4260</v>
+      </c>
+      <c r="I4" s="107" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>288</v>
+      </c>
+      <c r="K4" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="L4" s="14" t="s">
+        <v>287</v>
+      </c>
+      <c r="M4" s="31" t="s">
+        <v>50</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M4"/>
   <sheetViews>
@@ -3255,7 +3417,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V14"/>
   <sheetViews>
@@ -5909,7 +6071,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO32"/>
   <sheetViews>
-    <sheetView topLeftCell="AC1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="AL19" sqref="AL19"/>
     </sheetView>
   </sheetViews>
@@ -8292,7 +8454,7 @@
   <dimension ref="A2:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J4" sqref="J4"/>
+      <selection activeCell="K4" sqref="A2:K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
f/ntatum-TestingCmdWindowAbilities: Update to high alt documentation
Updated high altitude validation table and markdown
Also made dehydration fix in scenario file
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/EnergyEnvironmentValidation.xlsx
+++ b/share/doc/validation/Scenarios/EnergyEnvironmentValidation.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntatum\BioGearsCMake\core\share\doc\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ntatum\BioGearsCMake\master\share\doc\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="24720" windowHeight="10965" firstSheet="4" activeTab="10"/>
+    <workbookView xWindow="480" yWindow="120" windowWidth="24720" windowHeight="10965" firstSheet="4" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -1529,7 +1529,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="110">
+  <cellXfs count="111">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1634,9 +1634,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="3" borderId="1" xfId="2" applyNumberFormat="1" applyBorder="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1665,9 +1662,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="2">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1852,6 +1846,15 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="45" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="3" fillId="4" borderId="1" xfId="3" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2214,540 +2217,540 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.42578125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="22.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.28515625" style="69" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.140625" style="69"/>
+    <col min="1" max="1" width="1.7109375" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" style="67" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" style="67" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="67" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="63" t="s">
+    <row r="1" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A1" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C1" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="62" t="s">
+      <c r="C1" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="E1" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="56" t="s">
+      <c r="E1" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="G1" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="56" t="s">
+      <c r="G1" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="I1" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="56" t="s">
+      <c r="I1" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="55" t="s">
+      <c r="K1" s="53" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A2" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="54" t="s">
+      <c r="A2" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="52" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="61" t="s">
+      <c r="A3" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="59" t="s">
         <v>27</v>
       </c>
-      <c r="C3" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="58" t="s">
+      <c r="C3" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="56" t="s">
         <v>29</v>
       </c>
-      <c r="E3" s="52" t="s">
+      <c r="E3" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F3" s="73">
+      <c r="F3" s="71">
         <v>17</v>
       </c>
-      <c r="G3" s="57" t="s">
+      <c r="G3" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H3" s="76">
+      <c r="H3" s="74">
         <v>2</v>
       </c>
-      <c r="I3" s="57" t="s">
+      <c r="I3" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J3" s="72">
+      <c r="J3" s="70">
         <v>5</v>
       </c>
-      <c r="K3" s="54" t="s">
+      <c r="K3" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="61" t="s">
+      <c r="A4" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="59" t="s">
         <v>28</v>
       </c>
-      <c r="C4" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="58" t="s">
+      <c r="C4" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="56" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="52" t="s">
+      <c r="E4" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F4" s="73">
+      <c r="F4" s="71">
         <v>2</v>
       </c>
-      <c r="G4" s="57" t="s">
+      <c r="G4" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H4" s="76">
+      <c r="H4" s="74">
         <v>0</v>
       </c>
-      <c r="I4" s="57" t="s">
+      <c r="I4" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J4" s="72">
+      <c r="J4" s="70">
         <v>4</v>
       </c>
-      <c r="K4" s="54" t="s">
+      <c r="K4" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="61" t="s">
+      <c r="A5" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="59" t="s">
         <v>124</v>
       </c>
-      <c r="C5" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="58" t="s">
+      <c r="C5" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="56" t="s">
         <v>127</v>
       </c>
-      <c r="E5" s="52" t="s">
+      <c r="E5" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F5" s="73">
+      <c r="F5" s="71">
         <v>86</v>
       </c>
-      <c r="G5" s="57" t="s">
+      <c r="G5" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H5" s="76">
+      <c r="H5" s="74">
         <v>2</v>
       </c>
-      <c r="I5" s="57" t="s">
+      <c r="I5" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J5" s="72">
+      <c r="J5" s="70">
         <v>32</v>
       </c>
-      <c r="K5" s="54" t="s">
+      <c r="K5" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="61" t="s">
+      <c r="A6" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="59" t="s">
         <v>125</v>
       </c>
-      <c r="C6" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="58" t="s">
+      <c r="C6" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="E6" s="52" t="s">
+      <c r="E6" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F6" s="73">
+      <c r="F6" s="71">
         <v>1</v>
       </c>
-      <c r="G6" s="57" t="s">
+      <c r="G6" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H6" s="76">
+      <c r="H6" s="74">
         <v>0</v>
       </c>
-      <c r="I6" s="57" t="s">
+      <c r="I6" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="72">
+      <c r="J6" s="70">
         <v>0</v>
       </c>
-      <c r="K6" s="54" t="s">
+      <c r="K6" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="69" t="s">
+      <c r="A7" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="67" t="s">
         <v>245</v>
       </c>
-      <c r="C7" s="69" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="108" t="s">
+      <c r="C7" s="67" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="106" t="s">
         <v>246</v>
       </c>
-      <c r="E7" s="52" t="s">
+      <c r="E7" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F7" s="73">
+      <c r="F7" s="71">
         <v>0</v>
       </c>
-      <c r="G7" s="57" t="s">
+      <c r="G7" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H7" s="76">
+      <c r="H7" s="74">
         <v>1</v>
       </c>
-      <c r="I7" s="57" t="s">
+      <c r="I7" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J7" s="72">
+      <c r="J7" s="70">
         <v>0</v>
       </c>
-      <c r="K7" s="54" t="s">
+      <c r="K7" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B8" s="61" t="s">
+      <c r="A8" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="59" t="s">
         <v>181</v>
       </c>
-      <c r="C8" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="58" t="s">
+      <c r="C8" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="56" t="s">
         <v>182</v>
       </c>
-      <c r="E8" s="52" t="s">
+      <c r="E8" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F8" s="73">
+      <c r="F8" s="71">
         <v>20</v>
       </c>
-      <c r="G8" s="57" t="s">
+      <c r="G8" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H8" s="76">
+      <c r="H8" s="74">
         <v>4</v>
       </c>
-      <c r="I8" s="57" t="s">
+      <c r="I8" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J8" s="72">
+      <c r="J8" s="70">
         <v>0</v>
       </c>
-      <c r="K8" s="54" t="s">
+      <c r="K8" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A9" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="61" t="s">
+      <c r="A9" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="59" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D9" s="58" t="s">
+      <c r="C9" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D9" s="56" t="s">
         <v>185</v>
       </c>
-      <c r="E9" s="52" t="s">
+      <c r="E9" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="73">
+      <c r="F9" s="71">
         <v>5</v>
       </c>
-      <c r="G9" s="57" t="s">
+      <c r="G9" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H9" s="76">
+      <c r="H9" s="74">
         <v>1</v>
       </c>
-      <c r="I9" s="57" t="s">
+      <c r="I9" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J9" s="72">
+      <c r="J9" s="70">
         <v>0</v>
       </c>
-      <c r="K9" s="54" t="s">
+      <c r="K9" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="10" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A10" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="61" t="s">
+      <c r="A10" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="59" t="s">
         <v>131</v>
       </c>
-      <c r="C10" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="58" t="s">
+      <c r="C10" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="56" t="s">
         <v>269</v>
       </c>
-      <c r="E10" s="52" t="s">
+      <c r="E10" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F10" s="73">
+      <c r="F10" s="71">
         <v>10</v>
       </c>
-      <c r="G10" s="57" t="s">
+      <c r="G10" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H10" s="76">
+      <c r="H10" s="74">
         <v>1</v>
       </c>
-      <c r="I10" s="57" t="s">
+      <c r="I10" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J10" s="72">
+      <c r="J10" s="70">
         <v>2</v>
       </c>
-      <c r="K10" s="54" t="s">
+      <c r="K10" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A11" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="83"/>
-      <c r="C11" s="82" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="84" t="s">
+      <c r="A11" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="81"/>
+      <c r="C11" s="80" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="82" t="s">
         <v>126</v>
       </c>
-      <c r="E11" s="82" t="s">
+      <c r="E11" s="80" t="s">
         <v>49</v>
       </c>
-      <c r="F11" s="85">
+      <c r="F11" s="83">
         <f>SUM(F3:F10)</f>
         <v>141</v>
       </c>
-      <c r="G11" s="86" t="s">
+      <c r="G11" s="84" t="s">
         <v>92</v>
       </c>
-      <c r="H11" s="87">
+      <c r="H11" s="85">
         <f>SUM(H3:H10)</f>
         <v>11</v>
       </c>
-      <c r="I11" s="86" t="s">
+      <c r="I11" s="84" t="s">
         <v>93</v>
       </c>
-      <c r="J11" s="88">
+      <c r="J11" s="86">
         <f>SUM(J3:J10)</f>
         <v>43</v>
       </c>
-      <c r="K11" s="89" t="s">
+      <c r="K11" s="87" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="B14" s="69" t="s">
+      <c r="B14" s="67" t="s">
         <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A15" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="63" t="s">
+      <c r="A15" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="B15" s="61" t="s">
         <v>25</v>
       </c>
-      <c r="C15" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="D15" s="62" t="s">
+      <c r="C15" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="D15" s="60" t="s">
         <v>26</v>
       </c>
-      <c r="E15" s="63" t="s">
-        <v>47</v>
-      </c>
-      <c r="F15" s="56" t="s">
+      <c r="E15" s="61" t="s">
+        <v>47</v>
+      </c>
+      <c r="F15" s="54" t="s">
         <v>121</v>
       </c>
-      <c r="G15" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="H15" s="56" t="s">
+      <c r="G15" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="H15" s="54" t="s">
         <v>122</v>
       </c>
-      <c r="I15" s="56" t="s">
-        <v>47</v>
-      </c>
-      <c r="J15" s="56" t="s">
+      <c r="I15" s="54" t="s">
+        <v>47</v>
+      </c>
+      <c r="J15" s="54" t="s">
         <v>123</v>
       </c>
-      <c r="K15" s="55" t="s">
+      <c r="K15" s="53" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A16" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B16" s="60" t="s">
-        <v>48</v>
-      </c>
-      <c r="C16" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D16" s="59" t="s">
-        <v>48</v>
-      </c>
-      <c r="E16" s="52" t="s">
+      <c r="A16" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B16" s="58" t="s">
+        <v>48</v>
+      </c>
+      <c r="C16" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16" s="57" t="s">
+        <v>48</v>
+      </c>
+      <c r="E16" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="G16" s="57" t="s">
+      <c r="F16" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="G16" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H16" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="I16" s="57" t="s">
+      <c r="H16" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J16" s="53" t="s">
-        <v>48</v>
-      </c>
-      <c r="K16" s="54" t="s">
+      <c r="J16" s="51" t="s">
+        <v>48</v>
+      </c>
+      <c r="K16" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A17" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="B17" s="61" t="s">
+      <c r="A17" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="59" t="s">
         <v>132</v>
       </c>
-      <c r="C17" s="61" t="s">
-        <v>47</v>
-      </c>
-      <c r="D17" s="58"/>
-      <c r="E17" s="52" t="s">
+      <c r="C17" s="59" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="56"/>
+      <c r="E17" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F17" s="73"/>
-      <c r="G17" s="57" t="s">
+      <c r="F17" s="71"/>
+      <c r="G17" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H17" s="76"/>
-      <c r="I17" s="57" t="s">
+      <c r="H17" s="74"/>
+      <c r="I17" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J17" s="72"/>
-      <c r="K17" s="54" t="s">
+      <c r="J17" s="70"/>
+      <c r="K17" s="52" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="13.9" x14ac:dyDescent="0.3">
-      <c r="A18" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="77"/>
-      <c r="C18" s="52" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="68" t="s">
+      <c r="A18" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="75"/>
+      <c r="C18" s="50" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="66" t="s">
         <v>126</v>
       </c>
-      <c r="E18" s="52" t="s">
+      <c r="E18" s="50" t="s">
         <v>49</v>
       </c>
-      <c r="F18" s="70">
+      <c r="F18" s="68">
         <f>SUM(F17:F17)</f>
         <v>0</v>
       </c>
-      <c r="G18" s="57" t="s">
+      <c r="G18" s="55" t="s">
         <v>92</v>
       </c>
-      <c r="H18" s="74">
+      <c r="H18" s="72">
         <f>SUM(H17:H17)</f>
         <v>0</v>
       </c>
-      <c r="I18" s="57" t="s">
+      <c r="I18" s="55" t="s">
         <v>93</v>
       </c>
-      <c r="J18" s="72">
+      <c r="J18" s="70">
         <f>SUM(J17:J17)</f>
         <v>0</v>
       </c>
-      <c r="K18" s="54" t="s">
+      <c r="K18" s="52" t="s">
         <v>50</v>
       </c>
     </row>
@@ -2771,353 +2774,353 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.28515625" style="69" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="69" customWidth="1"/>
-    <col min="7" max="7" width="3" style="69" customWidth="1"/>
-    <col min="8" max="8" width="18.140625" style="69" customWidth="1"/>
-    <col min="9" max="9" width="4.42578125" style="69" customWidth="1"/>
-    <col min="10" max="10" width="16.140625" style="69" customWidth="1"/>
-    <col min="11" max="11" width="4" style="69" customWidth="1"/>
-    <col min="12" max="12" width="21.85546875" style="69" customWidth="1"/>
-    <col min="13" max="13" width="5.42578125" style="69" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" style="69" customWidth="1"/>
-    <col min="15" max="15" width="5.7109375" style="69" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.42578125" style="69" customWidth="1"/>
-    <col min="18" max="18" width="16" style="69" customWidth="1"/>
-    <col min="19" max="19" width="5" style="69" customWidth="1"/>
-    <col min="20" max="20" width="12" style="69" customWidth="1"/>
-    <col min="21" max="21" width="3.28515625" style="69" customWidth="1"/>
-    <col min="22" max="22" width="13.5703125" style="69" customWidth="1"/>
-    <col min="23" max="23" width="3.28515625" style="69" customWidth="1"/>
-    <col min="24" max="24" width="13.5703125" style="69" customWidth="1"/>
-    <col min="25" max="25" width="2.7109375" style="69" customWidth="1"/>
-    <col min="26" max="26" width="12.85546875" style="69" customWidth="1"/>
-    <col min="27" max="27" width="3.5703125" style="69" customWidth="1"/>
-    <col min="28" max="28" width="13" style="69" customWidth="1"/>
-    <col min="29" max="29" width="3" style="69" customWidth="1"/>
-    <col min="30" max="30" width="14.5703125" style="69" customWidth="1"/>
-    <col min="31" max="31" width="3.85546875" style="69" customWidth="1"/>
-    <col min="32" max="32" width="14" style="69" customWidth="1"/>
-    <col min="33" max="33" width="4" style="69" customWidth="1"/>
-    <col min="34" max="34" width="43.28515625" style="69" customWidth="1"/>
-    <col min="35" max="16384" width="9.140625" style="69"/>
+    <col min="1" max="1" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="67" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="67" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="67" customWidth="1"/>
+    <col min="7" max="7" width="3" style="67" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="67" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="67" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="67" customWidth="1"/>
+    <col min="11" max="11" width="4" style="67" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" style="67" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="67" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="67" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="67" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" style="67" customWidth="1"/>
+    <col min="18" max="18" width="16" style="67" customWidth="1"/>
+    <col min="19" max="19" width="5" style="67" customWidth="1"/>
+    <col min="20" max="20" width="12" style="67" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" style="67" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" style="67" customWidth="1"/>
+    <col min="23" max="23" width="3.28515625" style="67" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" style="67" customWidth="1"/>
+    <col min="25" max="25" width="2.7109375" style="67" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="67" customWidth="1"/>
+    <col min="27" max="27" width="3.5703125" style="67" customWidth="1"/>
+    <col min="28" max="28" width="13" style="67" customWidth="1"/>
+    <col min="29" max="29" width="3" style="67" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" style="67" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" style="67" customWidth="1"/>
+    <col min="32" max="32" width="14" style="67" customWidth="1"/>
+    <col min="33" max="33" width="4" style="67" customWidth="1"/>
+    <col min="34" max="34" width="43.28515625" style="67" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:34" ht="51" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="78" t="s">
+      <c r="A2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="78" t="s">
+      <c r="C2" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="78" t="s">
+      <c r="E2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="79" t="s">
+      <c r="G2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="77" t="s">
         <v>248</v>
       </c>
-      <c r="I2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="79" t="s">
+      <c r="I2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="77" t="s">
         <v>251</v>
       </c>
-      <c r="K2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="79" t="s">
+      <c r="K2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="77" t="s">
         <v>249</v>
       </c>
-      <c r="M2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="79" t="s">
+      <c r="M2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="77" t="s">
         <v>281</v>
       </c>
-      <c r="O2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="79" t="s">
+      <c r="O2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="77" t="s">
         <v>130</v>
       </c>
-      <c r="Q2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="79" t="s">
+      <c r="Q2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="S2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="79" t="s">
+      <c r="S2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" s="77" t="s">
         <v>270</v>
       </c>
-      <c r="U2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="V2" s="79" t="s">
+      <c r="U2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="77" t="s">
         <v>256</v>
       </c>
-      <c r="W2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="79" t="s">
+      <c r="W2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="77" t="s">
         <v>267</v>
       </c>
-      <c r="Y2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z2" s="79" t="s">
+      <c r="Y2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z2" s="77" t="s">
         <v>259</v>
       </c>
-      <c r="AA2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB2" s="79" t="s">
+      <c r="AA2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB2" s="77" t="s">
         <v>261</v>
       </c>
-      <c r="AC2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD2" s="79" t="s">
+      <c r="AC2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD2" s="77" t="s">
         <v>263</v>
       </c>
-      <c r="AE2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF2" s="79" t="s">
+      <c r="AE2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF2" s="77" t="s">
         <v>265</v>
       </c>
-      <c r="AG2" s="71" t="s">
+      <c r="AG2" s="69" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:34" x14ac:dyDescent="0.2">
-      <c r="A3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="P3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="Z3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="AA3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AB3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="AC3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AD3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="AE3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AF3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="AG3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="AH3" s="75"/>
+      <c r="A3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="Z3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="AA3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AB3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="AC3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AD3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="AE3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AF3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="AG3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="AH3" s="73"/>
     </row>
     <row r="4" spans="1:34" ht="255.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="78" t="s">
+      <c r="A4" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>247</v>
       </c>
-      <c r="C4" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="78" t="s">
+      <c r="C4" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>252</v>
       </c>
-      <c r="E4" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="78">
+      <c r="E4" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="76">
         <v>60</v>
       </c>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="69" t="s">
         <v>49</v>
       </c>
       <c r="H4" s="14" t="s">
         <v>258</v>
       </c>
-      <c r="I4" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="91" t="s">
+      <c r="I4" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="89" t="s">
         <v>250</v>
       </c>
-      <c r="K4" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="L4" s="91" t="s">
+      <c r="K4" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="L4" s="89" t="s">
         <v>257</v>
       </c>
-      <c r="M4" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="N4" s="91" t="s">
+      <c r="M4" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="N4" s="89" t="s">
         <v>253</v>
       </c>
-      <c r="O4" s="78" t="s">
+      <c r="O4" s="76" t="s">
         <v>93</v>
       </c>
       <c r="P4" s="32" t="s">
         <v>254</v>
       </c>
-      <c r="Q4" s="78" t="s">
+      <c r="Q4" s="76" t="s">
         <v>51</v>
       </c>
       <c r="R4" s="33" t="s">
         <v>271</v>
       </c>
-      <c r="S4" s="78" t="s">
+      <c r="S4" s="76" t="s">
         <v>51</v>
       </c>
       <c r="T4" s="33" t="s">
         <v>272</v>
       </c>
-      <c r="U4" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="V4" s="91" t="s">
+      <c r="U4" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="V4" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="W4" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="X4" s="91" t="s">
+      <c r="W4" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="X4" s="89" t="s">
         <v>268</v>
       </c>
-      <c r="Y4" s="78" t="s">
+      <c r="Y4" s="76" t="s">
         <v>51</v>
       </c>
       <c r="Z4" s="33" t="s">
         <v>260</v>
       </c>
-      <c r="AA4" s="78" t="s">
+      <c r="AA4" s="76" t="s">
         <v>93</v>
       </c>
-      <c r="AB4" s="109" t="s">
+      <c r="AB4" s="107" t="s">
         <v>262</v>
       </c>
-      <c r="AC4" s="78" t="s">
+      <c r="AC4" s="76" t="s">
         <v>51</v>
       </c>
       <c r="AD4" s="33" t="s">
         <v>264</v>
       </c>
-      <c r="AE4" s="78" t="s">
+      <c r="AE4" s="76" t="s">
         <v>92</v>
       </c>
       <c r="AF4" s="9" t="s">
         <v>266</v>
       </c>
-      <c r="AG4" s="78" t="s">
+      <c r="AG4" s="76" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="V5" s="48"/>
-      <c r="X5" s="48"/>
+      <c r="V5" s="46"/>
+      <c r="X5" s="46"/>
     </row>
     <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
-      <c r="Q9" s="48"/>
+      <c r="Q9" s="46"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3128,7 +3131,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:M4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
@@ -3138,37 +3141,37 @@
       <c r="A2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="39" t="s">
         <v>284</v>
       </c>
       <c r="K2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="L2" s="40" t="s">
+      <c r="L2" s="39" t="s">
         <v>285</v>
       </c>
       <c r="M2" s="31" t="s">
@@ -3241,7 +3244,7 @@
       <c r="H4" s="11">
         <v>4260</v>
       </c>
-      <c r="I4" s="107" t="s">
+      <c r="I4" s="105" t="s">
         <v>105</v>
       </c>
       <c r="J4" s="14" t="s">
@@ -3272,142 +3275,142 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.140625" style="69" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.42578125" style="69" customWidth="1"/>
-    <col min="5" max="5" width="1.85546875" style="69" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="22" style="69" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.7109375" style="69" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.42578125" style="69" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5703125" style="69" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.140625" style="69"/>
+    <col min="1" max="1" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="67" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="22" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" style="67" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="78" t="s">
+      <c r="A2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="76" t="s">
         <v>129</v>
       </c>
-      <c r="C2" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="78" t="s">
+      <c r="C2" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="76" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="78" t="s">
+      <c r="E2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="76" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="79" t="s">
+      <c r="G2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="77" t="s">
         <v>274</v>
       </c>
-      <c r="I2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="79" t="s">
+      <c r="I2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="77" t="s">
         <v>275</v>
       </c>
-      <c r="K2" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="79" t="s">
+      <c r="K2" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="77" t="s">
         <v>276</v>
       </c>
-      <c r="M2" s="71" t="s">
+      <c r="M2" s="69" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="A3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="80" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="71" t="s">
+      <c r="A3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="78" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="69" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="4" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="78" t="s">
+      <c r="A4" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="76" t="s">
         <v>273</v>
       </c>
-      <c r="C4" s="78" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="78" t="s">
+      <c r="C4" s="76" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="76" t="s">
         <v>279</v>
       </c>
-      <c r="E4" s="71" t="s">
-        <v>47</v>
-      </c>
-      <c r="F4" s="78">
+      <c r="E4" s="69" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="76">
         <v>60</v>
       </c>
-      <c r="G4" s="71" t="s">
+      <c r="G4" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="H4" s="91" t="s">
+      <c r="H4" s="89" t="s">
         <v>277</v>
       </c>
-      <c r="I4" s="78" t="s">
-        <v>51</v>
-      </c>
-      <c r="J4" s="91" t="s">
+      <c r="I4" s="76" t="s">
+        <v>51</v>
+      </c>
+      <c r="J4" s="89" t="s">
         <v>278</v>
       </c>
-      <c r="K4" s="78" t="s">
+      <c r="K4" s="76" t="s">
         <v>51</v>
       </c>
       <c r="L4" s="14" t="s">
         <v>277</v>
       </c>
-      <c r="M4" s="78" t="s">
+      <c r="M4" s="76" t="s">
         <v>50</v>
       </c>
     </row>
@@ -3442,585 +3445,585 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A1" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="42" t="s">
+      <c r="A1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="41" t="s">
         <v>238</v>
       </c>
-      <c r="C1" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D1" s="42" t="s">
+      <c r="C1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D1" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F1" s="42" t="s">
+      <c r="E1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F1" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H1" s="42" t="s">
+      <c r="G1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H1" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I1" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J1" s="104" t="s">
+      <c r="I1" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J1" s="102" t="s">
         <v>223</v>
       </c>
-      <c r="K1" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L1" s="42" t="s">
+      <c r="K1" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="M1" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N1" s="42" t="s">
+      <c r="M1" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N1" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="O1" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="P1" s="104" t="s">
+      <c r="O1" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="102" t="s">
         <v>226</v>
       </c>
-      <c r="Q1" s="104" t="s">
-        <v>47</v>
-      </c>
-      <c r="R1" s="104" t="s">
+      <c r="Q1" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="R1" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="S1" s="104" t="s">
-        <v>47</v>
-      </c>
-      <c r="T1" s="104"/>
-      <c r="U1" s="48"/>
-      <c r="V1" s="104" t="s">
+      <c r="S1" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="T1" s="102"/>
+      <c r="U1" s="46"/>
+      <c r="V1" s="102" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="2" spans="1:22" ht="33.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="E2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="G2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="I2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="K2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="M2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="O2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="S2" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="48"/>
+      <c r="A2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="E2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="G2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="K2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="M2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="O2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="S2" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" s="46"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="93" t="s">
+      <c r="V2" s="91" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="3" spans="1:22" ht="56.25" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="93" t="s">
+      <c r="A3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="91" t="s">
         <v>187</v>
       </c>
-      <c r="C3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="93" t="s">
+      <c r="C3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="91" t="s">
         <v>188</v>
       </c>
-      <c r="E3" s="42" t="s">
+      <c r="E3" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F3" s="1">
         <v>30</v>
       </c>
-      <c r="G3" s="42" t="s">
+      <c r="G3" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H3" s="1">
         <v>1200</v>
       </c>
-      <c r="I3" s="42" t="s">
+      <c r="I3" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J3" s="94" t="s">
+      <c r="J3" s="92" t="s">
         <v>189</v>
       </c>
-      <c r="K3" s="42" t="s">
+      <c r="K3" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L3" s="95" t="s">
+      <c r="L3" s="93" t="s">
         <v>191</v>
       </c>
-      <c r="M3" s="42" t="s">
+      <c r="M3" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N3" s="95" t="s">
+      <c r="N3" s="93" t="s">
         <v>192</v>
       </c>
-      <c r="O3" s="42" t="s">
+      <c r="O3" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="P3" s="95" t="s">
+      <c r="P3" s="93" t="s">
         <v>193</v>
       </c>
-      <c r="Q3" s="42" t="s">
+      <c r="Q3" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="R3" s="96" t="s">
+      <c r="R3" s="94" t="s">
         <v>193</v>
       </c>
-      <c r="S3" s="42" t="s">
+      <c r="S3" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T3" s="1"/>
       <c r="U3" s="1"/>
-      <c r="V3" s="93" t="s">
+      <c r="V3" s="91" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="4" spans="1:22" ht="68.25" x14ac:dyDescent="0.25">
-      <c r="A4" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="93" t="s">
+      <c r="A4" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="91" t="s">
         <v>195</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D4" s="93" t="s">
+      <c r="C4" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D4" s="91" t="s">
         <v>196</v>
       </c>
-      <c r="E4" s="42" t="s">
+      <c r="E4" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F4" s="1">
         <v>30</v>
       </c>
-      <c r="G4" s="42" t="s">
+      <c r="G4" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H4" s="1">
         <v>1100</v>
       </c>
-      <c r="I4" s="42" t="s">
+      <c r="I4" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J4" s="97" t="s">
+      <c r="J4" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="K4" s="42" t="s">
+      <c r="K4" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L4" s="98" t="s">
+      <c r="L4" s="96" t="s">
         <v>198</v>
       </c>
-      <c r="M4" s="42" t="s">
+      <c r="M4" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N4" s="99" t="s">
+      <c r="N4" s="97" t="s">
         <v>199</v>
       </c>
-      <c r="O4" s="42" t="s">
+      <c r="O4" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="P4" s="92" t="s">
+      <c r="P4" s="90" t="s">
         <v>201</v>
       </c>
-      <c r="Q4" s="42" t="s">
+      <c r="Q4" s="41" t="s">
         <v>200</v>
       </c>
       <c r="R4" s="9" t="s">
         <v>201</v>
       </c>
-      <c r="S4" s="42" t="s">
+      <c r="S4" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T4" s="1"/>
       <c r="U4" s="1"/>
-      <c r="V4" s="93" t="s">
+      <c r="V4" s="91" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="5" spans="1:22" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A5" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B5" s="93" t="s">
+      <c r="A5" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="91" t="s">
         <v>203</v>
       </c>
-      <c r="C5" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D5" s="93" t="s">
+      <c r="C5" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="91" t="s">
         <v>204</v>
       </c>
-      <c r="E5" s="42" t="s">
+      <c r="E5" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F5" s="1">
         <v>30</v>
       </c>
-      <c r="G5" s="42" t="s">
+      <c r="G5" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H5" s="1">
         <v>2700</v>
       </c>
-      <c r="I5" s="42" t="s">
+      <c r="I5" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="97" t="s">
+      <c r="J5" s="95" t="s">
         <v>197</v>
       </c>
-      <c r="K5" s="42" t="s">
+      <c r="K5" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L5" s="95" t="s">
+      <c r="L5" s="93" t="s">
         <v>198</v>
       </c>
-      <c r="M5" s="42" t="s">
+      <c r="M5" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N5" s="99" t="s">
+      <c r="N5" s="97" t="s">
         <v>205</v>
       </c>
-      <c r="O5" s="42" t="s">
+      <c r="O5" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="P5" s="100" t="s">
+      <c r="P5" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="Q5" s="42" t="s">
+      <c r="Q5" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="R5" s="100" t="s">
+      <c r="R5" s="98" t="s">
         <v>201</v>
       </c>
-      <c r="S5" s="42" t="s">
+      <c r="S5" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T5" s="1"/>
       <c r="U5" s="1"/>
-      <c r="V5" s="93" t="s">
+      <c r="V5" s="91" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:22" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A6" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B6" s="93" t="s">
+      <c r="A6" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B6" s="91" t="s">
         <v>207</v>
       </c>
-      <c r="C6" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D6" s="93" t="s">
+      <c r="C6" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D6" s="91" t="s">
         <v>208</v>
       </c>
-      <c r="E6" s="42" t="s">
+      <c r="E6" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F6" s="1">
         <v>30</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H6" s="1">
         <v>1500</v>
       </c>
-      <c r="I6" s="42" t="s">
+      <c r="I6" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J6" s="101" t="s">
+      <c r="J6" s="99" t="s">
         <v>209</v>
       </c>
-      <c r="K6" s="42" t="s">
+      <c r="K6" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L6" s="99" t="s">
+      <c r="L6" s="97" t="s">
         <v>210</v>
       </c>
-      <c r="M6" s="42" t="s">
+      <c r="M6" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N6" s="99" t="s">
+      <c r="N6" s="97" t="s">
         <v>211</v>
       </c>
-      <c r="O6" s="42" t="s">
+      <c r="O6" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="P6" s="100" t="s">
+      <c r="P6" s="98" t="s">
         <v>212</v>
       </c>
-      <c r="Q6" s="42" t="s">
+      <c r="Q6" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="R6" s="102" t="s">
+      <c r="R6" s="100" t="s">
         <v>213</v>
       </c>
-      <c r="S6" s="42" t="s">
+      <c r="S6" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T6" s="1"/>
       <c r="U6" s="1"/>
-      <c r="V6" s="93" t="s">
+      <c r="V6" s="91" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="7" spans="1:22" ht="75" x14ac:dyDescent="0.25">
-      <c r="A7" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B7" s="93" t="s">
+      <c r="A7" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="91" t="s">
         <v>215</v>
       </c>
-      <c r="C7" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" s="93" t="s">
+      <c r="C7" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D7" s="91" t="s">
         <v>216</v>
       </c>
-      <c r="E7" s="42" t="s">
+      <c r="E7" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F7" s="1">
         <v>30</v>
       </c>
-      <c r="G7" s="42" t="s">
+      <c r="G7" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H7" s="1">
         <v>1050</v>
       </c>
-      <c r="I7" s="42" t="s">
+      <c r="I7" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J7" s="103" t="s">
+      <c r="J7" s="101" t="s">
         <v>217</v>
       </c>
-      <c r="K7" s="42" t="s">
+      <c r="K7" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L7" s="99" t="s">
+      <c r="L7" s="97" t="s">
         <v>210</v>
       </c>
-      <c r="M7" s="42" t="s">
+      <c r="M7" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N7" s="99" t="s">
+      <c r="N7" s="97" t="s">
         <v>218</v>
       </c>
-      <c r="O7" s="42" t="s">
+      <c r="O7" s="41" t="s">
         <v>200</v>
       </c>
       <c r="P7" s="9" t="s">
         <v>212</v>
       </c>
-      <c r="Q7" s="42" t="s">
+      <c r="Q7" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="R7" s="99" t="s">
+      <c r="R7" s="97" t="s">
         <v>219</v>
       </c>
-      <c r="S7" s="42" t="s">
+      <c r="S7" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T7" s="1"/>
       <c r="U7" s="1"/>
-      <c r="V7" s="93" t="s">
+      <c r="V7" s="91" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="8" spans="1:22" ht="45" x14ac:dyDescent="0.25">
-      <c r="A8" s="48"/>
-      <c r="B8" s="48"/>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="M8" s="48"/>
-      <c r="N8" s="48"/>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
+      <c r="A8" s="46"/>
+      <c r="B8" s="46"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="46"/>
+      <c r="E8" s="46"/>
+      <c r="F8" s="46"/>
+      <c r="G8" s="46"/>
+      <c r="H8" s="46"/>
+      <c r="I8" s="46"/>
+      <c r="J8" s="46"/>
+      <c r="K8" s="46"/>
+      <c r="L8" s="46"/>
+      <c r="M8" s="46"/>
+      <c r="N8" s="46"/>
+      <c r="O8" s="46"/>
+      <c r="P8" s="46"/>
+      <c r="Q8" s="46"/>
+      <c r="R8" s="46"/>
+      <c r="S8" s="46"/>
       <c r="T8" s="1"/>
       <c r="U8" s="1"/>
-      <c r="V8" s="93" t="s">
+      <c r="V8" s="91" t="s">
         <v>221</v>
       </c>
     </row>
     <row r="9" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A9" s="48"/>
-      <c r="B9" s="48"/>
-      <c r="C9" s="48"/>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="48"/>
-      <c r="K9" s="48"/>
-      <c r="L9" s="48"/>
-      <c r="M9" s="48"/>
-      <c r="N9" s="48"/>
-      <c r="O9" s="48"/>
-      <c r="P9" s="48"/>
-      <c r="Q9" s="48"/>
-      <c r="R9" s="48"/>
-      <c r="S9" s="48"/>
+      <c r="A9" s="46"/>
+      <c r="B9" s="46"/>
+      <c r="C9" s="46"/>
+      <c r="D9" s="46"/>
+      <c r="E9" s="46"/>
+      <c r="F9" s="46"/>
+      <c r="G9" s="46"/>
+      <c r="H9" s="46"/>
+      <c r="I9" s="46"/>
+      <c r="J9" s="46"/>
+      <c r="K9" s="46"/>
+      <c r="L9" s="46"/>
+      <c r="M9" s="46"/>
+      <c r="N9" s="46"/>
+      <c r="O9" s="46"/>
+      <c r="P9" s="46"/>
+      <c r="Q9" s="46"/>
+      <c r="R9" s="46"/>
+      <c r="S9" s="46"/>
       <c r="T9" s="1"/>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
     <row r="10" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A10" s="48"/>
-      <c r="B10" s="48" t="s">
+      <c r="A10" s="46"/>
+      <c r="B10" s="46" t="s">
         <v>222</v>
       </c>
-      <c r="C10" s="48"/>
-      <c r="D10" s="48"/>
-      <c r="E10" s="48"/>
-      <c r="F10" s="48"/>
-      <c r="G10" s="48"/>
-      <c r="H10" s="48"/>
-      <c r="I10" s="48"/>
-      <c r="J10" s="48"/>
-      <c r="K10" s="48"/>
-      <c r="L10" s="48"/>
-      <c r="M10" s="48"/>
-      <c r="N10" s="48"/>
-      <c r="O10" s="48"/>
-      <c r="P10" s="48"/>
-      <c r="Q10" s="48"/>
-      <c r="R10" s="48"/>
-      <c r="S10" s="48"/>
+      <c r="C10" s="46"/>
+      <c r="D10" s="46"/>
+      <c r="E10" s="46"/>
+      <c r="F10" s="46"/>
+      <c r="G10" s="46"/>
+      <c r="H10" s="46"/>
+      <c r="I10" s="46"/>
+      <c r="J10" s="46"/>
+      <c r="K10" s="46"/>
+      <c r="L10" s="46"/>
+      <c r="M10" s="46"/>
+      <c r="N10" s="46"/>
+      <c r="O10" s="46"/>
+      <c r="P10" s="46"/>
+      <c r="Q10" s="46"/>
+      <c r="R10" s="46"/>
+      <c r="S10" s="46"/>
       <c r="T10" s="1"/>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
     <row r="11" spans="1:22" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="42" t="s">
+      <c r="A11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="42" t="s">
+      <c r="C11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="42" t="s">
+      <c r="E11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="42" t="s">
+      <c r="G11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="104" t="s">
+      <c r="I11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="102" t="s">
         <v>223</v>
       </c>
-      <c r="K11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="42" t="s">
+      <c r="K11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="41" t="s">
         <v>224</v>
       </c>
-      <c r="M11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N11" s="42" t="s">
+      <c r="M11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" s="41" t="s">
         <v>225</v>
       </c>
-      <c r="O11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="P11" s="104" t="s">
+      <c r="O11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="P11" s="102" t="s">
         <v>226</v>
       </c>
-      <c r="Q11" s="104" t="s">
-        <v>47</v>
-      </c>
-      <c r="R11" s="104" t="s">
+      <c r="Q11" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="R11" s="102" t="s">
         <v>227</v>
       </c>
-      <c r="S11" s="104" t="s">
+      <c r="S11" s="102" t="s">
         <v>47</v>
       </c>
       <c r="T11" s="1"/>
@@ -4028,61 +4031,61 @@
       <c r="V11" s="1"/>
     </row>
     <row r="12" spans="1:22" x14ac:dyDescent="0.25">
-      <c r="A12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="B12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="C12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="D12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="E12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="F12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="H12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="I12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="J12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="K12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="L12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="M12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="N12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="O12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="P12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q12" s="105" t="s">
-        <v>47</v>
-      </c>
-      <c r="R12" s="106" t="s">
-        <v>48</v>
-      </c>
-      <c r="S12" s="105" t="s">
+      <c r="A12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="B12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="D12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="F12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="J12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="K12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="L12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="M12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="N12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="O12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="P12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q12" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="R12" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="S12" s="103" t="s">
         <v>47</v>
       </c>
       <c r="T12" s="1"/>
@@ -4090,61 +4093,61 @@
       <c r="V12" s="1"/>
     </row>
     <row r="13" spans="1:22" ht="67.5" x14ac:dyDescent="0.2">
-      <c r="A13" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="93" t="s">
+      <c r="A13" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B13" s="91" t="s">
         <v>228</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="D13" s="93" t="s">
+      <c r="D13" s="91" t="s">
         <v>229</v>
       </c>
-      <c r="E13" s="42" t="s">
+      <c r="E13" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F13" s="1">
         <v>30</v>
       </c>
-      <c r="G13" s="42" t="s">
+      <c r="G13" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H13" s="1">
         <v>1530</v>
       </c>
-      <c r="I13" s="42" t="s">
+      <c r="I13" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J13" s="99" t="s">
+      <c r="J13" s="97" t="s">
         <v>209</v>
       </c>
-      <c r="K13" s="42" t="s">
+      <c r="K13" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L13" s="99" t="s">
+      <c r="L13" s="97" t="s">
         <v>210</v>
       </c>
-      <c r="M13" s="42" t="s">
+      <c r="M13" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N13" s="99" t="s">
+      <c r="N13" s="97" t="s">
         <v>211</v>
       </c>
-      <c r="O13" s="42" t="s">
+      <c r="O13" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="P13" s="100" t="s">
+      <c r="P13" s="98" t="s">
         <v>230</v>
       </c>
-      <c r="Q13" s="42" t="s">
+      <c r="Q13" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="R13" s="102" t="s">
+      <c r="R13" s="100" t="s">
         <v>231</v>
       </c>
-      <c r="S13" s="42" t="s">
+      <c r="S13" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T13" s="1"/>
@@ -4152,59 +4155,59 @@
       <c r="V13" s="1"/>
     </row>
     <row r="14" spans="1:22" ht="45" x14ac:dyDescent="0.2">
-      <c r="A14" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B14" s="93" t="s">
+      <c r="A14" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B14" s="91" t="s">
         <v>232</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>47</v>
       </c>
       <c r="D14" s="1"/>
-      <c r="E14" s="42" t="s">
+      <c r="E14" s="41" t="s">
         <v>47</v>
       </c>
       <c r="F14" s="1">
         <v>1530</v>
       </c>
-      <c r="G14" s="42" t="s">
+      <c r="G14" s="41" t="s">
         <v>47</v>
       </c>
       <c r="H14" s="1">
         <v>2430</v>
       </c>
-      <c r="I14" s="42" t="s">
+      <c r="I14" s="41" t="s">
         <v>49</v>
       </c>
-      <c r="J14" s="99" t="s">
+      <c r="J14" s="97" t="s">
         <v>233</v>
       </c>
-      <c r="K14" s="42" t="s">
+      <c r="K14" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="L14" s="99" t="s">
+      <c r="L14" s="97" t="s">
         <v>234</v>
       </c>
-      <c r="M14" s="42" t="s">
+      <c r="M14" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="N14" s="99" t="s">
+      <c r="N14" s="97" t="s">
         <v>235</v>
       </c>
-      <c r="O14" s="42" t="s">
+      <c r="O14" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="P14" s="99" t="s">
+      <c r="P14" s="97" t="s">
         <v>236</v>
       </c>
-      <c r="Q14" s="42" t="s">
+      <c r="Q14" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="R14" s="99" t="s">
+      <c r="R14" s="97" t="s">
         <v>237</v>
       </c>
-      <c r="S14" s="42" t="s">
+      <c r="S14" s="41" t="s">
         <v>50</v>
       </c>
       <c r="T14" s="1"/>
@@ -4232,57 +4235,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="B1" s="66" t="s">
+      <c r="A1" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="64" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="64" t="s">
+      <c r="C1" s="62" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="65" t="s">
-        <v>48</v>
-      </c>
-      <c r="C2" s="64" t="s">
+      <c r="A2" s="62" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="63" t="s">
+        <v>48</v>
+      </c>
+      <c r="C2" s="62" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="62" t="s">
         <v>49</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>117</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="62" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="62" t="s">
         <v>118</v>
       </c>
-      <c r="B4" s="81" t="s">
+      <c r="B4" s="79" t="s">
         <v>119</v>
       </c>
-      <c r="C4" s="64" t="s">
+      <c r="C4" s="62" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="64" t="s">
+      <c r="A5" s="62" t="s">
         <v>114</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>120</v>
       </c>
-      <c r="C5" s="64" t="s">
+      <c r="C5" s="62" t="s">
         <v>50</v>
       </c>
     </row>
@@ -4301,120 +4304,120 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.42578125" style="49" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.140625" style="49" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="23" style="49" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.140625" style="49" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.140625" style="49" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="49" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.28515625" style="49" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="9" style="49" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="49"/>
+    <col min="1" max="1" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="23" style="47" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" style="47" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" style="47" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="9" style="47" bestFit="1" customWidth="1"/>
+    <col min="16" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="B1" s="49" t="s">
+      <c r="B1" s="47" t="s">
         <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="42" t="s">
+      <c r="G2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="42" t="s">
+      <c r="I2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="K2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="42" t="s">
+      <c r="K2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="M2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="42" t="s">
+      <c r="M2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="40" t="s">
+      <c r="A3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4655,7 +4658,7 @@
     </row>
     <row r="9" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A9" s="4"/>
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="47" t="s">
         <v>138</v>
       </c>
       <c r="C9" s="4"/>
@@ -4664,101 +4667,101 @@
       <c r="F9" s="4"/>
       <c r="G9" s="4"/>
       <c r="H9" s="4"/>
-      <c r="J9" s="90"/>
-      <c r="L9" s="90"/>
-      <c r="N9" s="90"/>
+      <c r="J9" s="88"/>
+      <c r="L9" s="88"/>
+      <c r="N9" s="88"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A10" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C10" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D10" s="42" t="s">
+      <c r="C10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D10" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E10" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F10" s="42" t="s">
+      <c r="E10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F10" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G10" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H10" s="42" t="s">
+      <c r="G10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H10" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I10" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J10" s="42" t="s">
+      <c r="I10" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J10" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="K10" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="42" t="s">
+      <c r="K10" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="M10" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N10" s="42" t="s">
+      <c r="M10" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N10" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="O10" s="40" t="s">
+      <c r="O10" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I11" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="K11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="M11" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N11" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="O11" s="40" t="s">
+      <c r="A11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I11" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M11" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N11" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="O11" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -4910,7 +4913,7 @@
     </row>
     <row r="17" spans="1:15" x14ac:dyDescent="0.2">
       <c r="A17" s="4"/>
-      <c r="B17" s="49" t="s">
+      <c r="B17" s="47" t="s">
         <v>141</v>
       </c>
       <c r="C17" s="4"/>
@@ -4919,101 +4922,101 @@
       <c r="F17" s="4"/>
       <c r="G17" s="4"/>
       <c r="H17" s="4"/>
-      <c r="J17" s="90"/>
-      <c r="L17" s="90"/>
-      <c r="N17" s="90"/>
+      <c r="J17" s="88"/>
+      <c r="L17" s="88"/>
+      <c r="N17" s="88"/>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A18" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C18" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D18" s="42" t="s">
+      <c r="C18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E18" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F18" s="42" t="s">
+      <c r="E18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G18" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H18" s="42" t="s">
+      <c r="G18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I18" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J18" s="42" t="s">
+      <c r="I18" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="41" t="s">
         <v>168</v>
       </c>
-      <c r="K18" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L18" s="42" t="s">
+      <c r="K18" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="M18" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N18" s="42" t="s">
+      <c r="M18" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="41" t="s">
         <v>162</v>
       </c>
-      <c r="O18" s="40" t="s">
+      <c r="O18" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="K19" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="M19" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N19" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="O19" s="40" t="s">
+      <c r="A19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K19" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M19" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N19" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="O19" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5092,7 +5095,7 @@
       <c r="I21" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="J21" s="48" t="s">
+      <c r="J21" s="46" t="s">
         <v>170</v>
       </c>
       <c r="K21" s="31" t="s">
@@ -5112,12 +5115,12 @@
       </c>
     </row>
     <row r="23" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N23" s="51" t="s">
+      <c r="N23" s="49" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="24" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="N24" s="49">
+      <c r="N24" s="47">
         <f>100 * (12/(850/5.6))</f>
         <v>7.905882352941175</v>
       </c>
@@ -5154,96 +5157,96 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="42" t="s">
+      <c r="G2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="42" t="s">
+      <c r="I2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="41" t="s">
         <v>153</v>
       </c>
-      <c r="K2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="42" t="s">
+      <c r="K2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="M2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="42" t="s">
+      <c r="M2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="41" t="s">
         <v>156</v>
       </c>
-      <c r="O2" s="40" t="s">
+      <c r="O2" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="40" t="s">
+      <c r="A3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5322,7 +5325,7 @@
       <c r="I5" s="31" t="s">
         <v>49</v>
       </c>
-      <c r="J5" s="92" t="s">
+      <c r="J5" s="90" t="s">
         <v>158</v>
       </c>
       <c r="K5" s="31" t="s">
@@ -5386,157 +5389,157 @@
     <col min="26" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" s="46" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
-      <c r="A2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" s="42" t="s">
+    <row r="2" spans="1:30" s="45" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D2" s="42" t="s">
+      <c r="C2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="E2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F2" s="42" t="s">
+      <c r="E2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H2" s="42" t="s">
+      <c r="G2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
-      <c r="I2" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J2" s="42" t="s">
+      <c r="I2" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J2" s="41" t="s">
         <v>4</v>
       </c>
-      <c r="K2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L2" s="42" t="s">
+      <c r="K2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N2" s="42" t="s">
+      <c r="M2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N2" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="O2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="P2" s="42" t="s">
+      <c r="O2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="P2" s="41" t="s">
         <v>6</v>
       </c>
-      <c r="Q2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="R2" s="42" t="s">
+      <c r="Q2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="R2" s="41" t="s">
         <v>7</v>
       </c>
-      <c r="S2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="T2" s="42" t="s">
+      <c r="S2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="T2" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="U2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="V2" s="42" t="s">
+      <c r="U2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="V2" s="41" t="s">
         <v>9</v>
       </c>
-      <c r="W2" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="X2" s="42" t="s">
+      <c r="W2" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="X2" s="41" t="s">
         <v>11</v>
       </c>
-      <c r="Y2" s="40" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="3" spans="1:30" s="46" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="B3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="C3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="D3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="E3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="G3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="H3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="I3" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="J3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="K3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="L3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="M3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="N3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="O3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="P3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="R3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="S3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="T3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="U3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="V3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="W3" s="40" t="s">
-        <v>47</v>
-      </c>
-      <c r="X3" s="43" t="s">
-        <v>48</v>
-      </c>
-      <c r="Y3" s="40" t="s">
+      <c r="Y2" s="39" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:30" s="45" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="E3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="G3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="K3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="M3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="O3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="P3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="R3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="S3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="T3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="U3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="V3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="W3" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="X3" s="42" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y3" s="39" t="s">
         <v>47</v>
       </c>
     </row>
@@ -5616,11 +5619,11 @@
       <c r="Y4" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="Z4" s="39"/>
-      <c r="AA4" s="37"/>
-      <c r="AB4" s="37"/>
-      <c r="AC4" s="37"/>
-      <c r="AD4" s="37"/>
+      <c r="Z4" s="38"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
+      <c r="AC4" s="36"/>
+      <c r="AD4" s="36"/>
     </row>
     <row r="5" spans="1:30" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
@@ -5649,7 +5652,7 @@
       <c r="I5" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="J5" s="50" t="s">
+      <c r="J5" s="48" t="s">
         <v>100</v>
       </c>
       <c r="K5" s="31" t="s">
@@ -5685,7 +5688,7 @@
       <c r="U5" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="V5" s="91" t="s">
+      <c r="V5" s="89" t="s">
         <v>103</v>
       </c>
       <c r="W5" s="31" t="s">
@@ -5760,7 +5763,7 @@
       <c r="U6" s="31" t="s">
         <v>51</v>
       </c>
-      <c r="V6" s="91" t="s">
+      <c r="V6" s="89" t="s">
         <v>103</v>
       </c>
       <c r="W6" s="31" t="s">
@@ -5809,8 +5812,8 @@
   </sheetPr>
   <dimension ref="A2:X8"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:U4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -5908,61 +5911,61 @@
       <c r="A3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="B3" s="38" t="s">
+      <c r="B3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="C3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="D3" s="38" t="s">
+      <c r="D3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="E3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="F3" s="38" t="s">
+      <c r="F3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="G3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="I3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="J3" s="38" t="s">
+      <c r="J3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="K3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="L3" s="38" t="s">
+      <c r="L3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="M3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="N3" s="38" t="s">
+      <c r="N3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="O3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="P3" s="38" t="s">
+      <c r="P3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="Q3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="R3" s="38" t="s">
+      <c r="R3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="S3" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="T3" s="38" t="s">
+      <c r="T3" s="37" t="s">
         <v>48</v>
       </c>
       <c r="U3" s="5" t="s">
@@ -5995,9 +5998,9 @@
         <v>950</v>
       </c>
       <c r="I4" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="J4" s="36" t="s">
+        <v>105</v>
+      </c>
+      <c r="J4" s="108" t="s">
         <v>108</v>
       </c>
       <c r="K4" s="31" t="s">
@@ -6007,9 +6010,9 @@
         <v>109</v>
       </c>
       <c r="M4" s="31" t="s">
-        <v>114</v>
-      </c>
-      <c r="N4" s="36" t="s">
+        <v>49</v>
+      </c>
+      <c r="N4" s="109" t="s">
         <v>110</v>
       </c>
       <c r="O4" s="31" t="s">
@@ -6019,37 +6022,37 @@
         <v>111</v>
       </c>
       <c r="Q4" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="R4" s="32" t="s">
+        <v>51</v>
+      </c>
+      <c r="R4" s="14" t="s">
         <v>112</v>
       </c>
       <c r="S4" s="31" t="s">
-        <v>93</v>
-      </c>
-      <c r="T4" s="47" t="s">
+        <v>51</v>
+      </c>
+      <c r="T4" s="110" t="s">
         <v>113</v>
       </c>
       <c r="U4" s="31" t="s">
         <v>50</v>
       </c>
-      <c r="V4" s="41"/>
-      <c r="W4" s="39"/>
-      <c r="X4" s="39"/>
+      <c r="V4" s="40"/>
+      <c r="W4" s="38"/>
+      <c r="X4" s="38"/>
     </row>
     <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
-      <c r="U5" s="44"/>
-      <c r="V5" s="37"/>
-      <c r="W5" s="37"/>
-      <c r="X5" s="37"/>
+      <c r="U5" s="43"/>
+      <c r="V5" s="36"/>
+      <c r="W5" s="36"/>
+      <c r="X5" s="36"/>
     </row>
     <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="4"/>
-      <c r="U6" s="44"/>
-      <c r="V6" s="37"/>
-      <c r="W6" s="37"/>
-      <c r="X6" s="37"/>
+      <c r="U6" s="43"/>
+      <c r="V6" s="36"/>
+      <c r="W6" s="36"/>
+      <c r="X6" s="36"/>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.2">
       <c r="B7" s="17"/>
@@ -6087,77 +6090,77 @@
     <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.7109375" style="48" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="46" customWidth="1"/>
     <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.42578125" style="48" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" style="46" customWidth="1"/>
     <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.42578125" style="48" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="46" customWidth="1"/>
     <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21" style="48" customWidth="1"/>
+    <col min="17" max="17" width="21" style="46" customWidth="1"/>
     <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.85546875" style="48" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="46" customWidth="1"/>
     <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.42578125" style="48" customWidth="1"/>
+    <col min="21" max="21" width="26.42578125" style="46" customWidth="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="17" style="48" customWidth="1"/>
+    <col min="23" max="23" width="17" style="46" customWidth="1"/>
     <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.28515625" style="48" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" style="46" customWidth="1"/>
     <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.42578125" style="48" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" style="46" customWidth="1"/>
     <col min="28" max="28" width="36.140625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.28515625" style="48" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="46" customWidth="1"/>
     <col min="30" max="30" width="25.85546875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.85546875" style="48" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" style="46" customWidth="1"/>
     <col min="32" max="32" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.42578125" style="48" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" style="46" customWidth="1"/>
     <col min="34" max="34" width="34" bestFit="1" customWidth="1"/>
-    <col min="35" max="35" width="34" style="48" customWidth="1"/>
+    <col min="35" max="35" width="34" style="46" customWidth="1"/>
     <col min="36" max="36" width="24.42578125" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.42578125" style="48" customWidth="1"/>
+    <col min="37" max="37" width="24.42578125" style="46" customWidth="1"/>
     <col min="38" max="38" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="49"/>
-      <c r="B1" s="49"/>
-      <c r="C1" s="49"/>
-      <c r="D1" s="49"/>
-      <c r="E1" s="49"/>
-      <c r="F1" s="49"/>
-      <c r="G1" s="49"/>
-      <c r="H1" s="49"/>
-      <c r="I1" s="49"/>
-      <c r="J1" s="49"/>
-      <c r="K1" s="49"/>
-      <c r="L1" s="49"/>
-      <c r="M1" s="49"/>
-      <c r="N1" s="49"/>
-      <c r="O1" s="49"/>
-      <c r="P1" s="49"/>
-      <c r="Q1" s="49"/>
-      <c r="R1" s="49"/>
-      <c r="S1" s="49"/>
-      <c r="T1" s="49"/>
-      <c r="U1" s="49"/>
-      <c r="V1" s="49"/>
-      <c r="W1" s="49"/>
-      <c r="X1" s="49"/>
-      <c r="Y1" s="49"/>
-      <c r="Z1" s="49"/>
-      <c r="AA1" s="49"/>
-      <c r="AB1" s="49"/>
-      <c r="AC1" s="49"/>
-      <c r="AD1" s="49"/>
-      <c r="AE1" s="49"/>
-      <c r="AF1" s="49"/>
-      <c r="AG1" s="49"/>
-      <c r="AH1" s="49"/>
-      <c r="AI1" s="49"/>
-      <c r="AJ1" s="49"/>
-      <c r="AK1" s="49"/>
-      <c r="AL1" s="49"/>
-      <c r="AM1" s="49"/>
-      <c r="AN1" s="49"/>
+      <c r="A1" s="47"/>
+      <c r="B1" s="47"/>
+      <c r="C1" s="47"/>
+      <c r="D1" s="47"/>
+      <c r="E1" s="47"/>
+      <c r="F1" s="47"/>
+      <c r="G1" s="47"/>
+      <c r="H1" s="47"/>
+      <c r="I1" s="47"/>
+      <c r="J1" s="47"/>
+      <c r="K1" s="47"/>
+      <c r="L1" s="47"/>
+      <c r="M1" s="47"/>
+      <c r="N1" s="47"/>
+      <c r="O1" s="47"/>
+      <c r="P1" s="47"/>
+      <c r="Q1" s="47"/>
+      <c r="R1" s="47"/>
+      <c r="S1" s="47"/>
+      <c r="T1" s="47"/>
+      <c r="U1" s="47"/>
+      <c r="V1" s="47"/>
+      <c r="W1" s="47"/>
+      <c r="X1" s="47"/>
+      <c r="Y1" s="47"/>
+      <c r="Z1" s="47"/>
+      <c r="AA1" s="47"/>
+      <c r="AB1" s="47"/>
+      <c r="AC1" s="47"/>
+      <c r="AD1" s="47"/>
+      <c r="AE1" s="47"/>
+      <c r="AF1" s="47"/>
+      <c r="AG1" s="47"/>
+      <c r="AH1" s="47"/>
+      <c r="AI1" s="47"/>
+      <c r="AJ1" s="47"/>
+      <c r="AK1" s="47"/>
+      <c r="AL1" s="47"/>
+      <c r="AM1" s="47"/>
+      <c r="AN1" s="47"/>
     </row>
     <row r="2" spans="1:41" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
@@ -6518,7 +6521,7 @@
       <c r="AM4" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AN4" s="49"/>
+      <c r="AN4" s="47"/>
     </row>
     <row r="5" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
@@ -6638,7 +6641,7 @@
       <c r="AM5" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AN5" s="49"/>
+      <c r="AN5" s="47"/>
     </row>
     <row r="6" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
@@ -6679,10 +6682,10 @@
       <c r="AJ6" s="18"/>
       <c r="AK6" s="21"/>
       <c r="AL6" s="12"/>
-      <c r="AM6" s="51"/>
-      <c r="AN6" s="51"/>
-    </row>
-    <row r="7" spans="1:41" s="48" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="AM6" s="49"/>
+      <c r="AN6" s="49"/>
+    </row>
+    <row r="7" spans="1:41" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>47</v>
       </c>
@@ -6800,7 +6803,7 @@
       <c r="AM7" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AN7" s="49"/>
+      <c r="AN7" s="47"/>
     </row>
     <row r="8" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
@@ -6920,7 +6923,7 @@
       <c r="AM8" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AN8" s="51"/>
+      <c r="AN8" s="49"/>
     </row>
     <row r="9" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
@@ -6980,7 +6983,7 @@
       <c r="S9" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="T9" s="45" t="s">
+      <c r="T9" s="44" t="s">
         <v>67</v>
       </c>
       <c r="U9" s="11" t="s">
@@ -7040,7 +7043,7 @@
       <c r="AM9" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AN9" s="49"/>
+      <c r="AN9" s="47"/>
     </row>
     <row r="10" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
@@ -7160,7 +7163,7 @@
       <c r="AM10" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AN10" s="49"/>
+      <c r="AN10" s="47"/>
     </row>
     <row r="11" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
@@ -7201,10 +7204,10 @@
       <c r="AJ11" s="18"/>
       <c r="AK11" s="21"/>
       <c r="AL11" s="12"/>
-      <c r="AM11" s="51"/>
-      <c r="AN11" s="51"/>
-    </row>
-    <row r="12" spans="1:41" s="48" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="AM11" s="49"/>
+      <c r="AN11" s="49"/>
+    </row>
+    <row r="12" spans="1:41" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>47</v>
       </c>
@@ -7322,7 +7325,7 @@
       <c r="AM12" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AN12" s="49"/>
+      <c r="AN12" s="47"/>
     </row>
     <row r="13" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
@@ -7442,7 +7445,7 @@
       <c r="AM13" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AN13" s="51"/>
+      <c r="AN13" s="49"/>
     </row>
     <row r="14" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
@@ -7562,7 +7565,7 @@
       <c r="AM14" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AN14" s="49"/>
+      <c r="AN14" s="47"/>
     </row>
     <row r="15" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
@@ -7682,7 +7685,7 @@
       <c r="AM15" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AN15" s="49"/>
+      <c r="AN15" s="47"/>
     </row>
     <row r="16" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
@@ -7723,10 +7726,10 @@
       <c r="AJ16" s="18"/>
       <c r="AK16" s="21"/>
       <c r="AL16" s="12"/>
-      <c r="AM16" s="51"/>
-      <c r="AN16" s="51"/>
-    </row>
-    <row r="17" spans="1:40" s="48" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
+      <c r="AM16" s="49"/>
+      <c r="AN16" s="49"/>
+    </row>
+    <row r="17" spans="1:40" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>47</v>
       </c>
@@ -7844,7 +7847,7 @@
       <c r="AM17" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AN17" s="49"/>
+      <c r="AN17" s="47"/>
     </row>
     <row r="18" spans="1:40" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
@@ -7964,7 +7967,7 @@
       <c r="AM18" s="24" t="s">
         <v>47</v>
       </c>
-      <c r="AN18" s="51"/>
+      <c r="AN18" s="49"/>
     </row>
     <row r="19" spans="1:40" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
@@ -8084,7 +8087,7 @@
       <c r="AM19" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="AN19" s="49"/>
+      <c r="AN19" s="47"/>
     </row>
     <row r="20" spans="1:40" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
@@ -8204,93 +8207,93 @@
       <c r="AM20" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="AN20" s="49"/>
+      <c r="AN20" s="47"/>
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A21" s="49"/>
-      <c r="B21" s="49"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="49"/>
-      <c r="J21" s="49"/>
-      <c r="K21" s="49"/>
-      <c r="L21" s="49"/>
-      <c r="M21" s="49"/>
-      <c r="N21" s="49"/>
-      <c r="O21" s="49"/>
-      <c r="P21" s="49"/>
-      <c r="Q21" s="49"/>
-      <c r="R21" s="49"/>
-      <c r="S21" s="49"/>
-      <c r="T21" s="49"/>
-      <c r="U21" s="49"/>
-      <c r="V21" s="49"/>
-      <c r="W21" s="49"/>
-      <c r="X21" s="49"/>
-      <c r="Y21" s="49"/>
-      <c r="Z21" s="49"/>
-      <c r="AA21" s="49"/>
-      <c r="AB21" s="49"/>
-      <c r="AC21" s="49"/>
-      <c r="AD21" s="49"/>
-      <c r="AE21" s="49"/>
-      <c r="AF21" s="49"/>
-      <c r="AG21" s="49"/>
-      <c r="AH21" s="49"/>
-      <c r="AI21" s="49"/>
-      <c r="AJ21" s="49"/>
-      <c r="AK21" s="49"/>
-      <c r="AL21" s="49"/>
-      <c r="AM21" s="49"/>
-      <c r="AN21" s="49"/>
+      <c r="A21" s="47"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="47"/>
+      <c r="D21" s="47"/>
+      <c r="E21" s="47"/>
+      <c r="F21" s="47"/>
+      <c r="G21" s="47"/>
+      <c r="H21" s="47"/>
+      <c r="I21" s="47"/>
+      <c r="J21" s="47"/>
+      <c r="K21" s="47"/>
+      <c r="L21" s="47"/>
+      <c r="M21" s="47"/>
+      <c r="N21" s="47"/>
+      <c r="O21" s="47"/>
+      <c r="P21" s="47"/>
+      <c r="Q21" s="47"/>
+      <c r="R21" s="47"/>
+      <c r="S21" s="47"/>
+      <c r="T21" s="47"/>
+      <c r="U21" s="47"/>
+      <c r="V21" s="47"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="47"/>
+      <c r="Y21" s="47"/>
+      <c r="Z21" s="47"/>
+      <c r="AA21" s="47"/>
+      <c r="AB21" s="47"/>
+      <c r="AC21" s="47"/>
+      <c r="AD21" s="47"/>
+      <c r="AE21" s="47"/>
+      <c r="AF21" s="47"/>
+      <c r="AG21" s="47"/>
+      <c r="AH21" s="47"/>
+      <c r="AI21" s="47"/>
+      <c r="AJ21" s="47"/>
+      <c r="AK21" s="47"/>
+      <c r="AL21" s="47"/>
+      <c r="AM21" s="47"/>
+      <c r="AN21" s="47"/>
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.2">
-      <c r="A22" s="49"/>
+      <c r="A22" s="47"/>
       <c r="B22" s="13" t="s">
         <v>45</v>
       </c>
       <c r="C22" s="13"/>
-      <c r="D22" s="49"/>
-      <c r="E22" s="49"/>
-      <c r="F22" s="49"/>
-      <c r="G22" s="49"/>
-      <c r="H22" s="49"/>
-      <c r="I22" s="49"/>
-      <c r="J22" s="49"/>
-      <c r="K22" s="49"/>
-      <c r="L22" s="49"/>
-      <c r="M22" s="49"/>
-      <c r="N22" s="49"/>
-      <c r="O22" s="49"/>
-      <c r="P22" s="49"/>
-      <c r="Q22" s="49"/>
-      <c r="R22" s="49"/>
-      <c r="S22" s="49"/>
-      <c r="T22" s="49"/>
-      <c r="U22" s="49"/>
-      <c r="V22" s="49"/>
-      <c r="W22" s="49"/>
-      <c r="X22" s="49"/>
-      <c r="Y22" s="49"/>
-      <c r="Z22" s="49"/>
-      <c r="AA22" s="49"/>
-      <c r="AB22" s="49"/>
-      <c r="AC22" s="49"/>
-      <c r="AD22" s="49"/>
-      <c r="AE22" s="49"/>
-      <c r="AF22" s="49"/>
-      <c r="AG22" s="49"/>
-      <c r="AH22" s="49"/>
-      <c r="AI22" s="49"/>
-      <c r="AJ22" s="49"/>
-      <c r="AK22" s="49"/>
-      <c r="AL22" s="49"/>
-      <c r="AM22" s="49"/>
-      <c r="AN22" s="49"/>
+      <c r="D22" s="47"/>
+      <c r="E22" s="47"/>
+      <c r="F22" s="47"/>
+      <c r="G22" s="47"/>
+      <c r="H22" s="47"/>
+      <c r="I22" s="47"/>
+      <c r="J22" s="47"/>
+      <c r="K22" s="47"/>
+      <c r="L22" s="47"/>
+      <c r="M22" s="47"/>
+      <c r="N22" s="47"/>
+      <c r="O22" s="47"/>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="47"/>
+      <c r="T22" s="47"/>
+      <c r="U22" s="47"/>
+      <c r="V22" s="47"/>
+      <c r="W22" s="47"/>
+      <c r="X22" s="47"/>
+      <c r="Y22" s="47"/>
+      <c r="Z22" s="47"/>
+      <c r="AA22" s="47"/>
+      <c r="AB22" s="47"/>
+      <c r="AC22" s="47"/>
+      <c r="AD22" s="47"/>
+      <c r="AE22" s="47"/>
+      <c r="AF22" s="47"/>
+      <c r="AG22" s="47"/>
+      <c r="AH22" s="47"/>
+      <c r="AI22" s="47"/>
+      <c r="AJ22" s="47"/>
+      <c r="AK22" s="47"/>
+      <c r="AL22" s="47"/>
+      <c r="AM22" s="47"/>
+      <c r="AN22" s="47"/>
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.2">
       <c r="B24" s="17"/>
@@ -8344,45 +8347,45 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2" style="48" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="2" style="48" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="2" style="48" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2" style="46" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="2" style="46" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="2" style="46" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.42578125" style="48" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="46" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>46</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="40" t="s">
+      <c r="H2" s="39" t="s">
         <v>37</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="48" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>47</v>
       </c>
@@ -8468,31 +8471,31 @@
       <c r="A2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="41" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="42" t="s">
+      <c r="D2" s="41" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="F2" s="42" t="s">
+      <c r="F2" s="41" t="s">
         <v>2</v>
       </c>
       <c r="G2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="H2" s="42" t="s">
+      <c r="H2" s="41" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="31" t="s">
         <v>47</v>
       </c>
-      <c r="J2" s="40" t="s">
+      <c r="J2" s="39" t="s">
         <v>242</v>
       </c>
       <c r="K2" s="31" t="s">
@@ -8559,7 +8562,7 @@
       <c r="H4" s="11">
         <v>3630</v>
       </c>
-      <c r="I4" s="107" t="s">
+      <c r="I4" s="105" t="s">
         <v>105</v>
       </c>
       <c r="J4" s="9" t="s">

</xml_diff>

<commit_message>
- abaird-sarin: starting on the patient events
- lots of changes for sarin, fixed tidal volume issues, still need to test other substances

- patching to include all pralidoxime patient events, patched the logging issue with pericardium

- updates to adjust patiet reaction time

- finalize mental status as a physiology request

- added all patient events relevent to Sarin, added thresholds, updated atropine, including validation data for the drug

- update to the patient assessments

- deleting some zip build files and adding atropne reversal for patient states

- Minor documentation updates

- updates to io library stuff
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/EnergyEnvironmentValidation.xlsx
+++ b/share/doc/validation/Scenarios/EnergyEnvironmentValidation.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="23127"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core\share\doc\validation\Scenarios\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\BioGears\biogears\core\share\doc\validation\Scenarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{51ED50AB-DEFD-4D6B-B96F-EDC9C250C63B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="120" windowWidth="24720" windowHeight="10968" firstSheet="3" activeTab="4"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" firstSheet="6" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
@@ -26,12 +27,22 @@
     <sheet name="Dehydration" sheetId="11" r:id="rId12"/>
     <sheet name="SarinNerveAgent" sheetId="15" r:id="rId13"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1659" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1731" uniqueCount="304">
   <si>
     <t>Action</t>
   </si>
@@ -914,11 +925,53 @@
   <si>
     <t>&lt;/span&gt;|&lt;span class="warningr"&gt;</t>
   </si>
+  <si>
+    <t xml:space="preserve"> Severe Sarin Aerosol, Concentration = 4 mg/m^3</t>
+  </si>
+  <si>
+    <t>Severe + Treatment (Atropine)</t>
+  </si>
+  <si>
+    <t>Atropine 4 mg Iv @cite gupta2009handbook</t>
+  </si>
+  <si>
+    <t>70-80% inhibited @cite leikin2002review</t>
+  </si>
+  <si>
+    <t>Nausea and Vomiting</t>
+  </si>
+  <si>
+    <t>Secretions</t>
+  </si>
+  <si>
+    <t>Diaphoresis</t>
+  </si>
+  <si>
+    <t>Urination and Diarrhea</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reversal </t>
+  </si>
+  <si>
+    <t>Reversal</t>
+  </si>
+  <si>
+    <t>Moderate Rhinorrhea, Salivation @cite lee2003clinical</t>
+  </si>
+  <si>
+    <t>Vomiting (at 50% ACHE inhibited @cite lee2003clinical)</t>
+  </si>
+  <si>
+    <t>Moderate Diaphoresis @cite lee2003clinical</t>
+  </si>
+  <si>
+    <t>Urinary Incontinence and Diarrhea (at 75% ACHE inhibited) @cite lee2003clinical</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="30" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1887,14 +1940,14 @@
     <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
     <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
     <cellStyle name="Bad" xfId="2" builtinId="27" customBuiltin="1"/>
-    <cellStyle name="Bad 2" xfId="43"/>
-    <cellStyle name="Bad 3" xfId="45"/>
+    <cellStyle name="Bad 2" xfId="43" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Bad 3" xfId="45" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Good" xfId="1" builtinId="26" customBuiltin="1"/>
-    <cellStyle name="Good 2" xfId="42"/>
-    <cellStyle name="Good 3" xfId="44"/>
+    <cellStyle name="Good 2" xfId="42" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="Good 3" xfId="44" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
     <cellStyle name="Heading 1" xfId="5" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="6" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="7" builtinId="18" customBuiltin="1"/>
@@ -1998,6 +2051,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -2033,6 +2103,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2208,7 +2295,7 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -2218,22 +2305,22 @@
       <selection sqref="A1:K11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="67" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="67" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="19" style="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="43.44140625" style="67" customWidth="1"/>
-    <col min="5" max="5" width="22.44140625" style="67" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="5.109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="30.33203125" style="67" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="3.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="11" max="16384" width="9.109375" style="67"/>
+    <col min="3" max="3" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="43.42578125" style="67" customWidth="1"/>
+    <col min="5" max="5" width="22.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="30.28515625" style="67" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="3.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" s="65" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="61" t="s">
         <v>47</v>
       </c>
@@ -2268,7 +2355,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A2" s="59" t="s">
         <v>47</v>
       </c>
@@ -2303,7 +2390,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="41.4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A3" s="59" t="s">
         <v>47</v>
       </c>
@@ -2338,7 +2425,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="59" t="s">
         <v>47</v>
       </c>
@@ -2373,7 +2460,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="59" t="s">
         <v>47</v>
       </c>
@@ -2408,7 +2495,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="27.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="59" t="s">
         <v>47</v>
       </c>
@@ -2443,7 +2530,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="67" t="s">
         <v>47</v>
       </c>
@@ -2478,7 +2565,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="20.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="59" t="s">
         <v>47</v>
       </c>
@@ -2513,7 +2600,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="59" t="s">
         <v>47</v>
       </c>
@@ -2548,7 +2635,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="59" t="s">
         <v>47</v>
       </c>
@@ -2583,7 +2670,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="80" t="s">
         <v>47</v>
       </c>
@@ -2619,12 +2706,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B14" s="67" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="61" t="s">
         <v>47</v>
       </c>
@@ -2659,7 +2746,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="59" t="s">
         <v>47</v>
       </c>
@@ -2694,7 +2781,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="59" t="s">
         <v>47</v>
       </c>
@@ -2721,7 +2808,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="50" t="s">
         <v>47</v>
       </c>
@@ -2768,53 +2855,53 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <dimension ref="A2:AH9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="AH35" sqref="AH35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" style="67" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="67" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.88671875" style="67" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" style="67" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="67" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" style="67" customWidth="1"/>
     <col min="7" max="7" width="3" style="67" customWidth="1"/>
-    <col min="8" max="8" width="18.109375" style="67" customWidth="1"/>
-    <col min="9" max="9" width="4.44140625" style="67" customWidth="1"/>
-    <col min="10" max="10" width="16.109375" style="67" customWidth="1"/>
+    <col min="8" max="8" width="18.140625" style="67" customWidth="1"/>
+    <col min="9" max="9" width="4.42578125" style="67" customWidth="1"/>
+    <col min="10" max="10" width="16.140625" style="67" customWidth="1"/>
     <col min="11" max="11" width="4" style="67" customWidth="1"/>
-    <col min="12" max="12" width="21.88671875" style="67" customWidth="1"/>
-    <col min="13" max="13" width="5.44140625" style="67" customWidth="1"/>
-    <col min="14" max="14" width="15.6640625" style="67" customWidth="1"/>
-    <col min="15" max="15" width="5.6640625" style="67" customWidth="1"/>
-    <col min="16" max="16" width="19.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="6.44140625" style="67" customWidth="1"/>
+    <col min="12" max="12" width="21.85546875" style="67" customWidth="1"/>
+    <col min="13" max="13" width="5.42578125" style="67" customWidth="1"/>
+    <col min="14" max="14" width="15.7109375" style="67" customWidth="1"/>
+    <col min="15" max="15" width="5.7109375" style="67" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="6.42578125" style="67" customWidth="1"/>
     <col min="18" max="18" width="16" style="67" customWidth="1"/>
     <col min="19" max="19" width="5" style="67" customWidth="1"/>
     <col min="20" max="20" width="12" style="67" customWidth="1"/>
-    <col min="21" max="21" width="3.33203125" style="67" customWidth="1"/>
-    <col min="22" max="22" width="13.5546875" style="67" customWidth="1"/>
-    <col min="23" max="23" width="3.33203125" style="67" customWidth="1"/>
-    <col min="24" max="24" width="13.5546875" style="67" customWidth="1"/>
-    <col min="25" max="25" width="2.6640625" style="67" customWidth="1"/>
-    <col min="26" max="26" width="12.88671875" style="67" customWidth="1"/>
-    <col min="27" max="27" width="3.5546875" style="67" customWidth="1"/>
+    <col min="21" max="21" width="3.28515625" style="67" customWidth="1"/>
+    <col min="22" max="22" width="13.5703125" style="67" customWidth="1"/>
+    <col min="23" max="23" width="3.28515625" style="67" customWidth="1"/>
+    <col min="24" max="24" width="13.5703125" style="67" customWidth="1"/>
+    <col min="25" max="25" width="2.7109375" style="67" customWidth="1"/>
+    <col min="26" max="26" width="12.85546875" style="67" customWidth="1"/>
+    <col min="27" max="27" width="3.5703125" style="67" customWidth="1"/>
     <col min="28" max="28" width="13" style="67" customWidth="1"/>
     <col min="29" max="29" width="3" style="67" customWidth="1"/>
-    <col min="30" max="30" width="14.5546875" style="67" customWidth="1"/>
-    <col min="31" max="31" width="3.88671875" style="67" customWidth="1"/>
+    <col min="30" max="30" width="14.5703125" style="67" customWidth="1"/>
+    <col min="31" max="31" width="3.85546875" style="67" customWidth="1"/>
     <col min="32" max="32" width="14" style="67" customWidth="1"/>
     <col min="33" max="33" width="4" style="67" customWidth="1"/>
-    <col min="34" max="34" width="43.33203125" style="67" customWidth="1"/>
-    <col min="35" max="16384" width="9.109375" style="67"/>
+    <col min="34" max="34" width="43.28515625" style="67" customWidth="1"/>
+    <col min="35" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:34" ht="55.2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:34" ht="51" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
         <v>47</v>
       </c>
@@ -2915,7 +3002,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:34" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:34" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
         <v>47</v>
       </c>
@@ -3017,7 +3104,7 @@
       </c>
       <c r="AH3" s="73"/>
     </row>
-    <row r="4" spans="1:34" ht="276" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:34" ht="255.75" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>47</v>
       </c>
@@ -3118,11 +3205,11 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:34" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="V5" s="46"/>
       <c r="X5" s="46"/>
     </row>
-    <row r="9" spans="1:34" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:34" ht="15" x14ac:dyDescent="0.25">
       <c r="Q9" s="46"/>
     </row>
   </sheetData>
@@ -3131,16 +3218,16 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:M4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="2" spans="1:13" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>47</v>
       </c>
@@ -3181,7 +3268,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>47</v>
       </c>
@@ -3222,7 +3309,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>47</v>
       </c>
@@ -3269,32 +3356,32 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <dimension ref="A2:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="24.109375" style="67" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.44140625" style="67" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="67" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.140625" style="67" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.42578125" style="67" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="67" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="22" style="67" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.6640625" style="67" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.44140625" style="67" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="30.44140625" style="67" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5546875" style="67" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="9.109375" style="67"/>
+    <col min="7" max="7" width="20.7109375" style="67" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="30.42578125" style="67" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="14.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5703125" style="67" bestFit="1" customWidth="1"/>
+    <col min="14" max="16384" width="9.140625" style="67"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="69" t="s">
         <v>47</v>
       </c>
@@ -3335,7 +3422,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="69" t="s">
         <v>47</v>
       </c>
@@ -3376,7 +3463,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="69" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" ht="77.25" x14ac:dyDescent="0.25">
       <c r="A4" s="69" t="s">
         <v>47</v>
       </c>
@@ -3424,30 +3511,30 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V14"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
+  <dimension ref="A1:V20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A17" sqref="A17:S20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="20.33203125" customWidth="1"/>
-    <col min="8" max="8" width="12.6640625" customWidth="1"/>
-    <col min="9" max="9" width="14.44140625" customWidth="1"/>
-    <col min="10" max="10" width="11.33203125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="16.33203125" customWidth="1"/>
+    <col min="2" max="2" width="20.28515625" customWidth="1"/>
+    <col min="8" max="8" width="12.7109375" customWidth="1"/>
+    <col min="9" max="9" width="14.42578125" customWidth="1"/>
+    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="16.28515625" customWidth="1"/>
     <col min="12" max="12" width="12" customWidth="1"/>
-    <col min="13" max="13" width="13.33203125" customWidth="1"/>
+    <col min="13" max="13" width="13.28515625" customWidth="1"/>
     <col min="14" max="14" width="16" customWidth="1"/>
-    <col min="15" max="15" width="14.6640625" customWidth="1"/>
+    <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="17" customWidth="1"/>
-    <col min="17" max="17" width="15.44140625" customWidth="1"/>
-    <col min="18" max="18" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="15.42578125" customWidth="1"/>
+    <col min="18" max="18" width="13.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A1" s="41" t="s">
         <v>47</v>
       </c>
@@ -3511,7 +3598,7 @@
         <v>239</v>
       </c>
     </row>
-    <row r="2" spans="1:22" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:22" ht="33.75" x14ac:dyDescent="0.25">
       <c r="A2" s="103" t="s">
         <v>47</v>
       </c>
@@ -3575,7 +3662,7 @@
         <v>240</v>
       </c>
     </row>
-    <row r="3" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="56.25" x14ac:dyDescent="0.2">
       <c r="A3" s="41" t="s">
         <v>47</v>
       </c>
@@ -3639,7 +3726,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="4" spans="1:22" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:22" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A4" s="41" t="s">
         <v>47</v>
       </c>
@@ -3703,7 +3790,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="5" spans="1:22" ht="61.2" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A5" s="41" t="s">
         <v>47</v>
       </c>
@@ -3747,9 +3834,9 @@
         <v>205</v>
       </c>
       <c r="O5" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="P5" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="P5" s="14" t="s">
         <v>201</v>
       </c>
       <c r="Q5" s="41" t="s">
@@ -3767,7 +3854,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="6" spans="1:22" ht="51" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="41" t="s">
         <v>47</v>
       </c>
@@ -3811,9 +3898,9 @@
         <v>211</v>
       </c>
       <c r="O6" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="P6" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="P6" s="14" t="s">
         <v>212</v>
       </c>
       <c r="Q6" s="41" t="s">
@@ -3831,7 +3918,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="7" spans="1:22" ht="72" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:22" ht="75" x14ac:dyDescent="0.25">
       <c r="A7" s="41" t="s">
         <v>47</v>
       </c>
@@ -3875,9 +3962,9 @@
         <v>218</v>
       </c>
       <c r="O7" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="P7" s="9" t="s">
+        <v>190</v>
+      </c>
+      <c r="P7" s="14" t="s">
         <v>212</v>
       </c>
       <c r="Q7" s="41" t="s">
@@ -3895,7 +3982,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="8" spans="1:22" ht="30.6" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:22" ht="45" x14ac:dyDescent="0.25">
       <c r="A8" s="46"/>
       <c r="B8" s="46"/>
       <c r="C8" s="46"/>
@@ -3921,7 +4008,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A9" s="46"/>
       <c r="B9" s="46"/>
       <c r="C9" s="46"/>
@@ -3945,7 +4032,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A10" s="46"/>
       <c r="B10" s="46" t="s">
         <v>222</v>
@@ -3971,7 +4058,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:22" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:22" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A11" s="41" t="s">
         <v>47</v>
       </c>
@@ -4033,7 +4120,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:22" x14ac:dyDescent="0.25">
       <c r="A12" s="103" t="s">
         <v>47</v>
       </c>
@@ -4095,7 +4182,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:22" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A13" s="41" t="s">
         <v>47</v>
       </c>
@@ -4139,9 +4226,9 @@
         <v>211</v>
       </c>
       <c r="O13" s="41" t="s">
-        <v>200</v>
-      </c>
-      <c r="P13" s="98" t="s">
+        <v>190</v>
+      </c>
+      <c r="P13" s="14" t="s">
         <v>230</v>
       </c>
       <c r="Q13" s="41" t="s">
@@ -4157,7 +4244,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:22" ht="40.799999999999997" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:22" ht="45" x14ac:dyDescent="0.2">
       <c r="A14" s="41" t="s">
         <v>47</v>
       </c>
@@ -4216,6 +4303,245 @@
       <c r="T14" s="1"/>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.25">
+      <c r="B16" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="17" spans="1:19" ht="33.75" x14ac:dyDescent="0.2">
+      <c r="A17" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D17" s="41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F17" s="41" t="s">
+        <v>2</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H17" s="41" t="s">
+        <v>3</v>
+      </c>
+      <c r="I17" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="J17" s="102" t="s">
+        <v>223</v>
+      </c>
+      <c r="K17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="L17" s="41" t="s">
+        <v>294</v>
+      </c>
+      <c r="M17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="N17" s="41" t="s">
+        <v>295</v>
+      </c>
+      <c r="O17" s="39" t="s">
+        <v>47</v>
+      </c>
+      <c r="P17" s="102" t="s">
+        <v>296</v>
+      </c>
+      <c r="Q17" s="102" t="s">
+        <v>47</v>
+      </c>
+      <c r="R17" s="102" t="s">
+        <v>297</v>
+      </c>
+      <c r="S17" s="102" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>47</v>
+      </c>
+      <c r="B18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="C18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="D18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="E18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="F18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="G18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="H18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="I18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="J18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="K18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="L18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="M18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="N18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="O18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="P18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q18" s="103" t="s">
+        <v>47</v>
+      </c>
+      <c r="R18" s="104" t="s">
+        <v>48</v>
+      </c>
+      <c r="S18" s="103" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:19" ht="68.25" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>47</v>
+      </c>
+      <c r="B19" s="91" t="s">
+        <v>290</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="D19" s="91" t="s">
+        <v>208</v>
+      </c>
+      <c r="E19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F19" s="1">
+        <v>30</v>
+      </c>
+      <c r="G19" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H19" s="1">
+        <v>1530</v>
+      </c>
+      <c r="I19" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J19" s="97" t="s">
+        <v>293</v>
+      </c>
+      <c r="K19" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="L19" s="97" t="s">
+        <v>301</v>
+      </c>
+      <c r="M19" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="N19" s="97" t="s">
+        <v>300</v>
+      </c>
+      <c r="O19" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="P19" s="14" t="s">
+        <v>302</v>
+      </c>
+      <c r="Q19" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="R19" s="100" t="s">
+        <v>303</v>
+      </c>
+      <c r="S19" s="41" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="20" spans="1:19" ht="22.5" x14ac:dyDescent="0.2">
+      <c r="A20" t="s">
+        <v>47</v>
+      </c>
+      <c r="B20" s="91" t="s">
+        <v>292</v>
+      </c>
+      <c r="C20" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="D20" s="1"/>
+      <c r="E20" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="F20" s="1">
+        <v>1530</v>
+      </c>
+      <c r="G20" s="41" t="s">
+        <v>47</v>
+      </c>
+      <c r="H20" s="1">
+        <v>2430</v>
+      </c>
+      <c r="I20" s="41" t="s">
+        <v>49</v>
+      </c>
+      <c r="J20" s="97" t="s">
+        <v>154</v>
+      </c>
+      <c r="K20" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="L20" s="97" t="s">
+        <v>298</v>
+      </c>
+      <c r="M20" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="N20" s="97" t="s">
+        <v>299</v>
+      </c>
+      <c r="O20" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="P20" s="97" t="s">
+        <v>299</v>
+      </c>
+      <c r="Q20" s="41" t="s">
+        <v>190</v>
+      </c>
+      <c r="R20" s="97" t="s">
+        <v>299</v>
+      </c>
+      <c r="S20" s="41" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4223,21 +4549,21 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection sqref="A1:C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="62" t="s">
         <v>47</v>
       </c>
@@ -4248,7 +4574,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="62" t="s">
         <v>47</v>
       </c>
@@ -4259,7 +4585,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="62" t="s">
         <v>49</v>
       </c>
@@ -4270,7 +4596,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="62" t="s">
         <v>118</v>
       </c>
@@ -4281,7 +4607,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="62" t="s">
         <v>114</v>
       </c>
@@ -4298,34 +4624,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:O24"/>
   <sheetViews>
     <sheetView topLeftCell="A11" workbookViewId="0">
       <selection activeCell="N13" sqref="N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="35.44140625" style="47" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" style="47" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="18.33203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="47" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" style="47" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="18.28515625" style="47" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="23" style="47" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="34.109375" style="47" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="34.109375" style="47" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" style="47" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="39.33203125" style="47" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="34.140625" style="47" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="34.140625" style="47" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="47" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="39.28515625" style="47" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="9" style="47" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.109375" style="47"/>
+    <col min="16" max="16384" width="9.140625" style="47"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="B1" s="47" t="s">
         <v>137</v>
       </c>
@@ -4424,7 +4750,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>47</v>
       </c>
@@ -4471,7 +4797,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>47</v>
       </c>
@@ -4518,7 +4844,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>47</v>
       </c>
@@ -4565,7 +4891,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>47</v>
       </c>
@@ -4612,7 +4938,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>47</v>
       </c>
@@ -4768,7 +5094,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>47</v>
       </c>
@@ -4815,7 +5141,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="13" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>47</v>
       </c>
@@ -4862,7 +5188,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="21.6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>47</v>
       </c>
@@ -4909,7 +5235,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:15" ht="67.5" x14ac:dyDescent="0.2">
       <c r="B16" s="21" t="s">
         <v>165</v>
       </c>
@@ -5023,7 +5349,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="1:15" ht="132.6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:15" ht="146.25" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>47</v>
       </c>
@@ -5070,7 +5396,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="21" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>47</v>
       </c>
@@ -5117,12 +5443,12 @@
         <v>50</v>
       </c>
     </row>
-    <row r="23" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N23" s="49" t="s">
         <v>280</v>
       </c>
     </row>
-    <row r="24" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:15" x14ac:dyDescent="0.25">
       <c r="N24" s="47">
         <f>100 * (12/(850/5.6))</f>
         <v>7.905882352941175</v>
@@ -5134,32 +5460,32 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A2:O5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" customWidth="1"/>
-    <col min="3" max="3" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" customWidth="1"/>
-    <col min="5" max="5" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" customWidth="1"/>
-    <col min="7" max="7" width="1.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" customWidth="1"/>
-    <col min="9" max="10" width="22.44140625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" customWidth="1"/>
+    <col min="9" max="10" width="22.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.6640625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:15" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:15" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>47</v>
       </c>
@@ -5253,7 +5579,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:15" ht="52.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="57" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>47</v>
       </c>
@@ -5300,7 +5626,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" ht="79.5" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>47</v>
       </c>
@@ -5353,46 +5679,46 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A2:AD14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2:Y6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.33203125" style="5" customWidth="1"/>
-    <col min="3" max="3" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.6640625" style="5" customWidth="1"/>
-    <col min="5" max="5" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.44140625" style="5" customWidth="1"/>
-    <col min="7" max="7" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.6640625" style="5" customWidth="1"/>
-    <col min="9" max="10" width="22.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.7109375" style="5" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.42578125" style="5" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.7109375" style="5" customWidth="1"/>
+    <col min="9" max="10" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="23" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="18.109375" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.44140625" style="5" customWidth="1"/>
-    <col min="22" max="22" width="24.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="27.33203125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="18.140625" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.42578125" style="5" customWidth="1"/>
+    <col min="22" max="22" width="24.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="27.28515625" style="5" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="26" max="16384" width="9.109375" style="5"/>
+    <col min="26" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:30" s="45" customFormat="1" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" s="45" customFormat="1" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A2" s="41" t="s">
         <v>47</v>
       </c>
@@ -5546,7 +5872,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:30" ht="120.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:30" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>47</v>
       </c>
@@ -5628,7 +5954,7 @@
       <c r="AC4" s="36"/>
       <c r="AD4" s="36"/>
     </row>
-    <row r="5" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:30" ht="45.75" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>47</v>
       </c>
@@ -5704,7 +6030,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="6" spans="1:30" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:30" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>47</v>
       </c>
@@ -5809,7 +6135,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
@@ -5819,33 +6145,33 @@
       <selection activeCell="A2" sqref="A2:U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="10.199999999999999" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.109375" style="5" customWidth="1"/>
-    <col min="3" max="3" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.140625" style="5" customWidth="1"/>
+    <col min="3" max="3" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="16" style="5" customWidth="1"/>
-    <col min="5" max="5" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="9" style="5" customWidth="1"/>
-    <col min="7" max="7" width="1.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="8" style="5" customWidth="1"/>
     <col min="9" max="9" width="22" style="5" customWidth="1"/>
-    <col min="10" max="10" width="21.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="21.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="39" style="5" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.33203125" style="5" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="29.44140625" style="5" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="22.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="29.6640625" style="5" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="36.5546875" style="5" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="29.42578125" style="5" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="22.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="29.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="36.5703125" style="5" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="9" style="5" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.109375" style="5"/>
+    <col min="22" max="16384" width="9.140625" style="5"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" ht="30.6" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:24" ht="33.75" x14ac:dyDescent="0.2">
       <c r="A2" s="11" t="s">
         <v>47</v>
       </c>
@@ -5975,7 +6301,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:24" ht="31.8" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" ht="34.5" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>47</v>
       </c>
@@ -6043,13 +6369,13 @@
       <c r="W4" s="38"/>
       <c r="X4" s="38"/>
     </row>
-    <row r="5" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="U5" s="43"/>
       <c r="V5" s="36"/>
       <c r="W5" s="36"/>
       <c r="X5" s="36"/>
     </row>
-    <row r="6" spans="1:24" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" ht="15" x14ac:dyDescent="0.25">
       <c r="B6" s="17"/>
       <c r="C6" s="4"/>
       <c r="U6" s="43"/>
@@ -6074,56 +6400,56 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:AO32"/>
   <sheetViews>
     <sheetView topLeftCell="AB11" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A17" sqref="A17:AM20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="1.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="10.33203125" customWidth="1"/>
-    <col min="3" max="3" width="1.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="1.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="1.88671875" style="7" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.6640625" style="7" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.6640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="25.6640625" style="46" customWidth="1"/>
-    <col min="12" max="12" width="27.44140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.44140625" style="46" customWidth="1"/>
-    <col min="14" max="14" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.44140625" style="46" customWidth="1"/>
+    <col min="1" max="1" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10.28515625" customWidth="1"/>
+    <col min="3" max="3" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="1.85546875" style="7" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.7109375" style="7" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="25.7109375" style="46" customWidth="1"/>
+    <col min="12" max="12" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.42578125" style="46" customWidth="1"/>
+    <col min="14" max="14" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.42578125" style="46" customWidth="1"/>
     <col min="16" max="16" width="21" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21" style="46" customWidth="1"/>
-    <col min="18" max="18" width="21.88671875" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.88671875" style="46" customWidth="1"/>
-    <col min="20" max="20" width="26.44140625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="26.44140625" style="46" customWidth="1"/>
+    <col min="18" max="18" width="21.85546875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="46" customWidth="1"/>
+    <col min="20" max="20" width="26.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="26.42578125" style="46" customWidth="1"/>
     <col min="22" max="22" width="17" bestFit="1" customWidth="1"/>
     <col min="23" max="23" width="17" style="46" customWidth="1"/>
-    <col min="24" max="24" width="19.33203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="19.33203125" style="46" customWidth="1"/>
-    <col min="26" max="26" width="19.44140625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="19.44140625" style="46" customWidth="1"/>
-    <col min="28" max="28" width="36.109375" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="13.33203125" style="46" customWidth="1"/>
-    <col min="30" max="30" width="25.88671875" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="25.88671875" style="46" customWidth="1"/>
-    <col min="32" max="32" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="15.44140625" style="46" customWidth="1"/>
+    <col min="24" max="24" width="19.28515625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="19.28515625" style="46" customWidth="1"/>
+    <col min="26" max="26" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.42578125" style="46" customWidth="1"/>
+    <col min="28" max="28" width="36.140625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" style="46" customWidth="1"/>
+    <col min="30" max="30" width="25.85546875" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="25.85546875" style="46" customWidth="1"/>
+    <col min="32" max="32" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="15.42578125" style="46" customWidth="1"/>
     <col min="34" max="34" width="34" bestFit="1" customWidth="1"/>
     <col min="35" max="35" width="34" style="46" customWidth="1"/>
-    <col min="36" max="36" width="24.44140625" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="24.44140625" style="46" customWidth="1"/>
-    <col min="38" max="38" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="24.42578125" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="24.42578125" style="46" customWidth="1"/>
+    <col min="38" max="38" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:41" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="47"/>
       <c r="B1" s="47"/>
       <c r="C1" s="47"/>
@@ -6165,7 +6491,7 @@
       <c r="AM1" s="47"/>
       <c r="AN1" s="47"/>
     </row>
-    <row r="2" spans="1:41" s="29" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:41" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A2" s="24" t="s">
         <v>47</v>
       </c>
@@ -6285,7 +6611,7 @@
       </c>
       <c r="AN2" s="25"/>
     </row>
-    <row r="3" spans="1:41" s="29" customFormat="1" ht="13.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:41" s="29" customFormat="1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A3" s="24" t="s">
         <v>47</v>
       </c>
@@ -6406,7 +6732,7 @@
       <c r="AN3" s="26"/>
       <c r="AO3" s="27"/>
     </row>
-    <row r="4" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A4" s="24" t="s">
         <v>47</v>
       </c>
@@ -6526,7 +6852,7 @@
       </c>
       <c r="AN4" s="47"/>
     </row>
-    <row r="5" spans="1:41" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A5" s="24" t="s">
         <v>47</v>
       </c>
@@ -6646,7 +6972,7 @@
       </c>
       <c r="AN5" s="47"/>
     </row>
-    <row r="6" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="22"/>
       <c r="B6" s="21"/>
       <c r="C6" s="21"/>
@@ -6688,7 +7014,7 @@
       <c r="AM6" s="49"/>
       <c r="AN6" s="49"/>
     </row>
-    <row r="7" spans="1:41" s="46" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:41" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A7" s="24" t="s">
         <v>47</v>
       </c>
@@ -6808,7 +7134,7 @@
       </c>
       <c r="AN7" s="47"/>
     </row>
-    <row r="8" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="35" t="s">
         <v>47</v>
       </c>
@@ -6928,7 +7254,7 @@
       </c>
       <c r="AN8" s="49"/>
     </row>
-    <row r="9" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A9" s="24" t="s">
         <v>47</v>
       </c>
@@ -7048,7 +7374,7 @@
       </c>
       <c r="AN9" s="47"/>
     </row>
-    <row r="10" spans="1:41" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="24" t="s">
         <v>47</v>
       </c>
@@ -7168,7 +7494,7 @@
       </c>
       <c r="AN10" s="47"/>
     </row>
-    <row r="11" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="22"/>
       <c r="B11" s="21"/>
       <c r="C11" s="21"/>
@@ -7210,7 +7536,7 @@
       <c r="AM11" s="49"/>
       <c r="AN11" s="49"/>
     </row>
-    <row r="12" spans="1:41" s="46" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:41" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A12" s="24" t="s">
         <v>47</v>
       </c>
@@ -7330,7 +7656,7 @@
       </c>
       <c r="AN12" s="47"/>
     </row>
-    <row r="13" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A13" s="35" t="s">
         <v>47</v>
       </c>
@@ -7450,7 +7776,7 @@
       </c>
       <c r="AN13" s="49"/>
     </row>
-    <row r="14" spans="1:41" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A14" s="24" t="s">
         <v>47</v>
       </c>
@@ -7570,7 +7896,7 @@
       </c>
       <c r="AN14" s="47"/>
     </row>
-    <row r="15" spans="1:41" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:41" ht="60" x14ac:dyDescent="0.25">
       <c r="A15" s="24" t="s">
         <v>47</v>
       </c>
@@ -7690,7 +8016,7 @@
       </c>
       <c r="AN15" s="47"/>
     </row>
-    <row r="16" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:41" s="34" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="22"/>
       <c r="B16" s="21"/>
       <c r="C16" s="21"/>
@@ -7732,7 +8058,7 @@
       <c r="AM16" s="49"/>
       <c r="AN16" s="49"/>
     </row>
-    <row r="17" spans="1:40" s="46" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:40" s="46" customFormat="1" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="24" t="s">
         <v>47</v>
       </c>
@@ -7852,7 +8178,7 @@
       </c>
       <c r="AN17" s="47"/>
     </row>
-    <row r="18" spans="1:40" s="34" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:40" s="34" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A18" s="35" t="s">
         <v>47</v>
       </c>
@@ -7972,7 +8298,7 @@
       </c>
       <c r="AN18" s="49"/>
     </row>
-    <row r="19" spans="1:40" ht="43.2" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:40" ht="60" x14ac:dyDescent="0.25">
       <c r="A19" s="24" t="s">
         <v>47</v>
       </c>
@@ -8092,7 +8418,7 @@
       </c>
       <c r="AN19" s="47"/>
     </row>
-    <row r="20" spans="1:40" ht="57.6" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:40" ht="60" x14ac:dyDescent="0.25">
       <c r="A20" s="24" t="s">
         <v>47</v>
       </c>
@@ -8212,7 +8538,7 @@
       </c>
       <c r="AN20" s="47"/>
     </row>
-    <row r="21" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A21" s="47"/>
       <c r="B21" s="47"/>
       <c r="C21" s="47"/>
@@ -8318,19 +8644,19 @@
       <c r="B28" s="17"/>
       <c r="C28" s="17"/>
     </row>
-    <row r="29" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
     </row>
-    <row r="30" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
     </row>
-    <row r="31" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B31" s="12"/>
       <c r="C31" s="12"/>
     </row>
-    <row r="32" spans="1:40" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:40" x14ac:dyDescent="0.25">
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
     </row>
@@ -8341,24 +8667,24 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <dimension ref="A1:I7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="2" style="46" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="2" style="46" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="2" style="46" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.44140625" style="46" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.42578125" style="46" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="1" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>47</v>
@@ -8388,7 +8714,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>47</v>
       </c>
@@ -8417,7 +8743,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:9" ht="62.4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" ht="68.25" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>47</v>
       </c>
@@ -8446,7 +8772,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B7" s="1"/>
       <c r="C7" s="1"/>
     </row>
@@ -8456,21 +8782,21 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A2:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="7" max="7" width="7" customWidth="1"/>
     <col min="8" max="8" width="13" customWidth="1"/>
-    <col min="9" max="9" width="10.6640625" customWidth="1"/>
+    <col min="9" max="9" width="10.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:11" ht="20.399999999999999" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" ht="22.5" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>47</v>
       </c>
@@ -8505,7 +8831,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3" s="31" t="s">
         <v>47</v>
       </c>
@@ -8540,7 +8866,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="72" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="75" x14ac:dyDescent="0.25">
       <c r="A4" s="31" t="s">
         <v>47</v>
       </c>

</xml_diff>